<commit_message>
More realistic spec file
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/2021_22_lettings_bulk_upload.xlsx
+++ b/spec/fixtures/files/2021_22_lettings_bulk_upload.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="301">
   <si>
     <t xml:space="preserve">Question</t>
   </si>
@@ -1281,10 +1281,49 @@
     <t xml:space="preserve">Field Number</t>
   </si>
   <si>
-    <t xml:space="preserve">T6745</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T9876</t>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E09000028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">439JOE005A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mt.data.gary.meyler@communities.gov.uk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E09000030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">439JOE001D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">439JOE006F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">439JOE001A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">439JOE008A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">439JOE006B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">439JOE008F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">439KOE007F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">439JOE001C</t>
   </si>
 </sst>
 </file>
@@ -1530,7 +1569,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1751,11 +1790,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1843,10 +1890,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:EC17"/>
+  <dimension ref="A1:EF17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3908,1382 +3955,2387 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55" t="s">
-        <v>286</v>
+        <v>2</v>
+      </c>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="56"/>
+      <c r="H7" s="55" t="n">
+        <v>4626</v>
       </c>
       <c r="I7" s="55" t="n">
         <v>2</v>
       </c>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
-      <c r="M7" s="55"/>
-      <c r="N7" s="55"/>
-      <c r="O7" s="55"/>
-      <c r="P7" s="55"/>
-      <c r="Q7" s="55"/>
-      <c r="R7" s="55"/>
-      <c r="S7" s="55"/>
-      <c r="T7" s="55"/>
-      <c r="U7" s="55"/>
-      <c r="V7" s="55"/>
-      <c r="W7" s="55"/>
-      <c r="X7" s="55"/>
-      <c r="Y7" s="55"/>
-      <c r="Z7" s="55"/>
-      <c r="AA7" s="55"/>
-      <c r="AB7" s="55"/>
-      <c r="AC7" s="55"/>
-      <c r="AD7" s="55"/>
-      <c r="AE7" s="55"/>
-      <c r="AF7" s="55"/>
-      <c r="AG7" s="55"/>
-      <c r="AH7" s="55"/>
-      <c r="AI7" s="55"/>
-      <c r="AJ7" s="55"/>
-      <c r="AK7" s="55"/>
-      <c r="AL7" s="55"/>
-      <c r="AM7" s="55"/>
-      <c r="AN7" s="55"/>
-      <c r="AO7" s="55"/>
-      <c r="AP7" s="55"/>
-      <c r="AQ7" s="55"/>
-      <c r="AR7" s="55"/>
-      <c r="AS7" s="55"/>
-      <c r="AT7" s="55"/>
-      <c r="AU7" s="55"/>
-      <c r="AV7" s="55"/>
-      <c r="AW7" s="55"/>
-      <c r="AX7" s="55"/>
-      <c r="AY7" s="55"/>
-      <c r="AZ7" s="55"/>
-      <c r="BA7" s="55"/>
-      <c r="BB7" s="55"/>
-      <c r="BC7" s="55"/>
-      <c r="BD7" s="55"/>
-      <c r="BE7" s="55"/>
-      <c r="BF7" s="55"/>
-      <c r="BG7" s="55"/>
-      <c r="BH7" s="55"/>
-      <c r="BI7" s="55"/>
-      <c r="BJ7" s="55"/>
-      <c r="BK7" s="55"/>
-      <c r="BL7" s="55"/>
-      <c r="BM7" s="55"/>
-      <c r="BN7" s="55"/>
-      <c r="BO7" s="55"/>
-      <c r="BP7" s="55"/>
-      <c r="BQ7" s="55"/>
-      <c r="BR7" s="55"/>
-      <c r="BS7" s="55"/>
-      <c r="BT7" s="55"/>
-      <c r="BU7" s="55"/>
-      <c r="BV7" s="55"/>
-      <c r="BW7" s="55"/>
-      <c r="BX7" s="55"/>
-      <c r="BY7" s="55"/>
-      <c r="BZ7" s="55"/>
-      <c r="CA7" s="55"/>
-      <c r="CB7" s="55"/>
-      <c r="CC7" s="55"/>
-      <c r="CD7" s="55"/>
-      <c r="CE7" s="55"/>
-      <c r="CF7" s="55"/>
-      <c r="CG7" s="55"/>
-      <c r="CH7" s="55"/>
-      <c r="CI7" s="55"/>
-      <c r="CJ7" s="55"/>
-      <c r="CK7" s="55"/>
-      <c r="CL7" s="55"/>
-      <c r="CM7" s="55"/>
-      <c r="CN7" s="55"/>
-      <c r="CO7" s="55"/>
-      <c r="CP7" s="55"/>
-      <c r="CQ7" s="55"/>
-      <c r="CR7" s="55"/>
-      <c r="CS7" s="55"/>
-      <c r="CT7" s="55"/>
-      <c r="CU7" s="55"/>
-      <c r="CV7" s="55"/>
-      <c r="CW7" s="55"/>
-      <c r="CX7" s="55"/>
-      <c r="CY7" s="55"/>
-      <c r="CZ7" s="55"/>
-      <c r="DA7" s="55"/>
-      <c r="DB7" s="55"/>
-      <c r="DC7" s="55"/>
-      <c r="DD7" s="55"/>
-      <c r="DE7" s="55"/>
-      <c r="DF7" s="55"/>
-      <c r="DG7" s="55"/>
-      <c r="DH7" s="55"/>
-      <c r="DI7" s="55"/>
-      <c r="DJ7" s="55"/>
-      <c r="DK7" s="55"/>
-      <c r="DL7" s="55"/>
-      <c r="DM7" s="55"/>
-      <c r="DN7" s="55"/>
-      <c r="DO7" s="55"/>
-      <c r="DP7" s="55"/>
-      <c r="DQ7" s="55"/>
-      <c r="DR7" s="55"/>
-      <c r="DS7" s="55"/>
-      <c r="DT7" s="55"/>
-      <c r="DU7" s="55"/>
-      <c r="DV7" s="55"/>
-      <c r="DW7" s="55"/>
-      <c r="DX7" s="55"/>
-      <c r="DY7" s="55"/>
-      <c r="DZ7" s="55"/>
-      <c r="EA7" s="55"/>
+      <c r="J7" s="55" t="n">
+        <v>5</v>
+      </c>
+      <c r="K7" s="56"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="55" t="n">
+        <v>47</v>
+      </c>
+      <c r="N7" s="56"/>
+      <c r="O7" s="56"/>
+      <c r="P7" s="56"/>
+      <c r="Q7" s="56"/>
+      <c r="R7" s="56"/>
+      <c r="S7" s="56"/>
+      <c r="T7" s="56"/>
+      <c r="U7" s="57" t="s">
+        <v>286</v>
+      </c>
+      <c r="V7" s="56"/>
+      <c r="W7" s="56"/>
+      <c r="X7" s="56"/>
+      <c r="Y7" s="56"/>
+      <c r="Z7" s="56"/>
+      <c r="AA7" s="56"/>
+      <c r="AB7" s="56"/>
+      <c r="AC7" s="56"/>
+      <c r="AD7" s="56"/>
+      <c r="AE7" s="56"/>
+      <c r="AF7" s="56"/>
+      <c r="AG7" s="56"/>
+      <c r="AH7" s="56"/>
+      <c r="AI7" s="56"/>
+      <c r="AJ7" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AK7" s="56"/>
+      <c r="AL7" s="56"/>
+      <c r="AM7" s="56"/>
+      <c r="AN7" s="56"/>
+      <c r="AO7" s="56"/>
+      <c r="AP7" s="56"/>
+      <c r="AQ7" s="56"/>
+      <c r="AR7" s="55" t="n">
+        <v>13</v>
+      </c>
+      <c r="AS7" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT7" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="AU7" s="56"/>
+      <c r="AV7" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW7" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX7" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AY7" s="56"/>
+      <c r="AZ7" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA7" s="55" t="n">
+        <v>34</v>
+      </c>
+      <c r="BB7" s="56"/>
+      <c r="BC7" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="BD7" s="56"/>
+      <c r="BE7" s="56"/>
+      <c r="BF7" s="56"/>
+      <c r="BG7" s="56"/>
+      <c r="BH7" s="56"/>
+      <c r="BI7" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ7" s="55" t="n">
+        <v>33</v>
+      </c>
+      <c r="BK7" s="57" t="s">
+        <v>287</v>
+      </c>
+      <c r="BL7" s="56"/>
+      <c r="BM7" s="56"/>
+      <c r="BN7" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO7" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="BP7" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="BQ7" s="55" t="n">
+        <v>7</v>
+      </c>
+      <c r="BR7" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BS7" s="56"/>
+      <c r="BT7" s="56"/>
+      <c r="BU7" s="56"/>
+      <c r="BV7" s="56"/>
+      <c r="BW7" s="56"/>
+      <c r="BX7" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BY7" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BZ7" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="CA7" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="CB7" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC7" s="55" t="n">
+        <v>90.44</v>
+      </c>
+      <c r="CD7" s="55" t="n">
+        <v>140.67</v>
+      </c>
+      <c r="CE7" s="55" t="n">
+        <v>5.34</v>
+      </c>
+      <c r="CF7" s="55" t="n">
+        <v>43</v>
+      </c>
+      <c r="CG7" s="55" t="n">
+        <v>279.45</v>
+      </c>
+      <c r="CH7" s="56"/>
+      <c r="CI7" s="56"/>
+      <c r="CJ7" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="CK7" s="56"/>
+      <c r="CL7" s="55" t="n">
+        <v>10</v>
+      </c>
+      <c r="CM7" s="55" t="n">
+        <v>8</v>
+      </c>
+      <c r="CN7" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="CO7" s="56"/>
+      <c r="CP7" s="56"/>
+      <c r="CQ7" s="56"/>
+      <c r="CR7" s="56"/>
+      <c r="CS7" s="55" t="n">
+        <v>17</v>
+      </c>
+      <c r="CT7" s="55" t="n">
+        <v>9</v>
+      </c>
+      <c r="CU7" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="CV7" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW7" s="57" t="s">
+        <v>288</v>
+      </c>
+      <c r="CX7" s="56"/>
+      <c r="CY7" s="56"/>
+      <c r="CZ7" s="56"/>
+      <c r="DA7" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="DB7" s="56"/>
+      <c r="DC7" s="55" t="n">
+        <v>12</v>
+      </c>
+      <c r="DD7" s="56"/>
+      <c r="DE7" s="56"/>
+      <c r="DF7" s="56"/>
+      <c r="DG7" s="56"/>
+      <c r="DH7" s="55" t="n">
+        <v>107242</v>
+      </c>
+      <c r="DI7" s="57" t="s">
+        <v>289</v>
+      </c>
+      <c r="DJ7" s="55" t="n">
+        <v>107242</v>
+      </c>
+      <c r="DK7" s="56"/>
+      <c r="DL7" s="57" t="s">
+        <v>288</v>
+      </c>
+      <c r="DM7" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DN7" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DO7" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DP7" s="56"/>
+      <c r="DQ7" s="56"/>
+      <c r="DR7" s="56"/>
+      <c r="DS7" s="56"/>
+      <c r="DT7" s="56"/>
+      <c r="DU7" s="56"/>
+      <c r="DV7" s="56"/>
+      <c r="DW7" s="56"/>
+      <c r="DX7" s="56"/>
+      <c r="DY7" s="56"/>
+      <c r="DZ7" s="56"/>
+      <c r="EA7" s="56"/>
+      <c r="EB7" s="56"/>
+      <c r="EC7" s="56"/>
+      <c r="ED7" s="56"/>
+      <c r="EE7" s="56"/>
+      <c r="EF7" s="56"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="56"/>
+      <c r="H8" s="55" t="n">
+        <v>4173</v>
+      </c>
+      <c r="I8" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="J8" s="55" t="n">
+        <v>5</v>
+      </c>
+      <c r="K8" s="56"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="57" t="s">
+        <v>290</v>
+      </c>
+      <c r="N8" s="56"/>
+      <c r="O8" s="56"/>
+      <c r="P8" s="56"/>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="56"/>
+      <c r="S8" s="56"/>
+      <c r="T8" s="56"/>
+      <c r="U8" s="57" t="s">
+        <v>290</v>
+      </c>
+      <c r="V8" s="56"/>
+      <c r="W8" s="56"/>
+      <c r="X8" s="56"/>
+      <c r="Y8" s="56"/>
+      <c r="Z8" s="56"/>
+      <c r="AA8" s="56"/>
+      <c r="AB8" s="56"/>
+      <c r="AC8" s="56"/>
+      <c r="AD8" s="56"/>
+      <c r="AE8" s="56"/>
+      <c r="AF8" s="56"/>
+      <c r="AG8" s="56"/>
+      <c r="AH8" s="56"/>
+      <c r="AI8" s="56"/>
+      <c r="AJ8" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="56"/>
+      <c r="AL8" s="56"/>
+      <c r="AM8" s="56"/>
+      <c r="AN8" s="56"/>
+      <c r="AO8" s="56"/>
+      <c r="AP8" s="56"/>
+      <c r="AQ8" s="56"/>
+      <c r="AR8" s="55" t="n">
+        <v>17</v>
+      </c>
+      <c r="AS8" s="55" t="n">
+        <v>13</v>
+      </c>
+      <c r="AT8" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU8" s="56"/>
+      <c r="AV8" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW8" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AX8" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AY8" s="56"/>
+      <c r="AZ8" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA8" s="55" t="n">
+        <v>28</v>
+      </c>
+      <c r="BB8" s="56"/>
+      <c r="BC8" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="BD8" s="56"/>
+      <c r="BE8" s="56"/>
+      <c r="BF8" s="56"/>
+      <c r="BG8" s="56"/>
+      <c r="BH8" s="56"/>
+      <c r="BI8" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ8" s="55" t="n">
+        <v>25</v>
+      </c>
+      <c r="BK8" s="57" t="s">
+        <v>291</v>
+      </c>
+      <c r="BL8" s="56"/>
+      <c r="BM8" s="56"/>
+      <c r="BN8" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO8" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="BP8" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="BQ8" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR8" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="BS8" s="56"/>
+      <c r="BT8" s="56"/>
+      <c r="BU8" s="56"/>
+      <c r="BV8" s="56"/>
+      <c r="BW8" s="56"/>
+      <c r="BX8" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BY8" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BZ8" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="CA8" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="CB8" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC8" s="55" t="n">
+        <v>90.44</v>
+      </c>
+      <c r="CD8" s="55" t="n">
+        <v>140.67</v>
+      </c>
+      <c r="CE8" s="55" t="n">
+        <v>5.34</v>
+      </c>
+      <c r="CF8" s="55" t="n">
+        <v>43</v>
+      </c>
+      <c r="CG8" s="55" t="n">
+        <v>279.45</v>
+      </c>
+      <c r="CH8" s="56"/>
+      <c r="CI8" s="56"/>
+      <c r="CJ8" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="CK8" s="56"/>
+      <c r="CL8" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="CM8" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="CN8" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="CO8" s="56"/>
+      <c r="CP8" s="56"/>
+      <c r="CQ8" s="56"/>
+      <c r="CR8" s="56"/>
+      <c r="CS8" s="55" t="n">
+        <v>22</v>
+      </c>
+      <c r="CT8" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="CU8" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="CV8" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW8" s="57" t="s">
+        <v>292</v>
+      </c>
+      <c r="CX8" s="56"/>
+      <c r="CY8" s="56"/>
+      <c r="CZ8" s="56"/>
+      <c r="DA8" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="DB8" s="56"/>
+      <c r="DC8" s="55" t="n">
+        <v>12</v>
+      </c>
+      <c r="DD8" s="56"/>
+      <c r="DE8" s="56"/>
+      <c r="DF8" s="56"/>
+      <c r="DG8" s="56"/>
+      <c r="DH8" s="55" t="n">
+        <v>107242</v>
+      </c>
+      <c r="DI8" s="57" t="s">
+        <v>289</v>
+      </c>
+      <c r="DJ8" s="55" t="n">
+        <v>107242</v>
+      </c>
+      <c r="DK8" s="56"/>
+      <c r="DL8" s="57" t="s">
+        <v>292</v>
+      </c>
+      <c r="DM8" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DN8" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DO8" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DP8" s="56"/>
+      <c r="DQ8" s="56"/>
+      <c r="DR8" s="56"/>
+      <c r="DS8" s="56"/>
+      <c r="DT8" s="56"/>
+      <c r="DU8" s="56"/>
+      <c r="DV8" s="56"/>
+      <c r="DW8" s="56"/>
+      <c r="DX8" s="56"/>
+      <c r="DY8" s="56"/>
+      <c r="DZ8" s="56"/>
+      <c r="EA8" s="56"/>
+      <c r="EB8" s="56"/>
+      <c r="EC8" s="56"/>
+      <c r="ED8" s="56"/>
+      <c r="EE8" s="56"/>
+      <c r="EF8" s="56"/>
+    </row>
+    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="56"/>
+      <c r="H9" s="55" t="n">
+        <v>4196</v>
+      </c>
+      <c r="I9" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" s="55" t="n">
+        <v>5</v>
+      </c>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="55" t="n">
+        <v>46</v>
+      </c>
+      <c r="N9" s="56"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="56"/>
+      <c r="S9" s="56"/>
+      <c r="T9" s="56"/>
+      <c r="U9" s="57" t="s">
+        <v>293</v>
+      </c>
+      <c r="V9" s="56"/>
+      <c r="W9" s="56"/>
+      <c r="X9" s="56"/>
+      <c r="Y9" s="56"/>
+      <c r="Z9" s="56"/>
+      <c r="AA9" s="56"/>
+      <c r="AB9" s="56"/>
+      <c r="AC9" s="56"/>
+      <c r="AD9" s="56"/>
+      <c r="AE9" s="56"/>
+      <c r="AF9" s="56"/>
+      <c r="AG9" s="56"/>
+      <c r="AH9" s="56"/>
+      <c r="AI9" s="56"/>
+      <c r="AJ9" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="AK9" s="56"/>
+      <c r="AL9" s="56"/>
+      <c r="AM9" s="56"/>
+      <c r="AN9" s="56"/>
+      <c r="AO9" s="56"/>
+      <c r="AP9" s="56"/>
+      <c r="AQ9" s="56"/>
+      <c r="AR9" s="55" t="n">
+        <v>7</v>
+      </c>
+      <c r="AS9" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT9" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="AU9" s="56"/>
+      <c r="AV9" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW9" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AX9" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AY9" s="56"/>
+      <c r="AZ9" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA9" s="55" t="n">
+        <v>28</v>
+      </c>
+      <c r="BB9" s="56"/>
+      <c r="BC9" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="BD9" s="56"/>
+      <c r="BE9" s="56"/>
+      <c r="BF9" s="56"/>
+      <c r="BG9" s="56"/>
+      <c r="BH9" s="56"/>
+      <c r="BI9" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ9" s="55" t="n">
+        <v>28</v>
+      </c>
+      <c r="BK9" s="57" t="s">
         <v>287</v>
       </c>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="55"/>
-      <c r="L8" s="55"/>
-      <c r="M8" s="55"/>
-      <c r="N8" s="55"/>
-      <c r="O8" s="55"/>
-      <c r="P8" s="55"/>
-      <c r="Q8" s="55"/>
-      <c r="R8" s="55"/>
-      <c r="S8" s="55"/>
-      <c r="T8" s="55"/>
-      <c r="U8" s="55"/>
-      <c r="V8" s="55"/>
-      <c r="W8" s="55"/>
-      <c r="X8" s="55"/>
-      <c r="Y8" s="55"/>
-      <c r="Z8" s="55"/>
-      <c r="AA8" s="55"/>
-      <c r="AB8" s="55"/>
-      <c r="AC8" s="55"/>
-      <c r="AD8" s="55"/>
-      <c r="AE8" s="55"/>
-      <c r="AF8" s="55"/>
-      <c r="AG8" s="55"/>
-      <c r="AH8" s="55"/>
-      <c r="AI8" s="55"/>
-      <c r="AJ8" s="55"/>
-      <c r="AK8" s="55"/>
-      <c r="AL8" s="55"/>
-      <c r="AM8" s="55"/>
-      <c r="AN8" s="55"/>
-      <c r="AO8" s="55"/>
-      <c r="AP8" s="55"/>
-      <c r="AQ8" s="55"/>
-      <c r="AR8" s="55"/>
-      <c r="AS8" s="55"/>
-      <c r="AT8" s="55"/>
-      <c r="AU8" s="55"/>
-      <c r="AV8" s="55"/>
-      <c r="AW8" s="55"/>
-      <c r="AX8" s="55"/>
-      <c r="AY8" s="55"/>
-      <c r="AZ8" s="55"/>
-      <c r="BA8" s="55"/>
-      <c r="BB8" s="55"/>
-      <c r="BC8" s="55"/>
-      <c r="BD8" s="55"/>
-      <c r="BE8" s="55"/>
-      <c r="BF8" s="55"/>
-      <c r="BG8" s="55"/>
-      <c r="BH8" s="55"/>
-      <c r="BI8" s="55"/>
-      <c r="BJ8" s="55"/>
-      <c r="BK8" s="55"/>
-      <c r="BL8" s="55"/>
-      <c r="BM8" s="55"/>
-      <c r="BN8" s="55"/>
-      <c r="BO8" s="55"/>
-      <c r="BP8" s="55"/>
-      <c r="BQ8" s="55"/>
-      <c r="BR8" s="55"/>
-      <c r="BS8" s="55"/>
-      <c r="BT8" s="55"/>
-      <c r="BU8" s="55"/>
-      <c r="BV8" s="55"/>
-      <c r="BW8" s="55"/>
-      <c r="BX8" s="55"/>
-      <c r="BY8" s="55"/>
-      <c r="BZ8" s="55"/>
-      <c r="CA8" s="55"/>
-      <c r="CB8" s="55"/>
-      <c r="CC8" s="55"/>
-      <c r="CD8" s="55"/>
-      <c r="CE8" s="55"/>
-      <c r="CF8" s="55"/>
-      <c r="CG8" s="55"/>
-      <c r="CH8" s="55"/>
-      <c r="CI8" s="55"/>
-      <c r="CJ8" s="55"/>
-      <c r="CK8" s="55"/>
-      <c r="CL8" s="55"/>
-      <c r="CM8" s="55"/>
-      <c r="CN8" s="55"/>
-      <c r="CO8" s="55"/>
-      <c r="CP8" s="55"/>
-      <c r="CQ8" s="55"/>
-      <c r="CR8" s="55"/>
-      <c r="CS8" s="55"/>
-      <c r="CT8" s="55"/>
-      <c r="CU8" s="55"/>
-      <c r="CV8" s="55"/>
-      <c r="CW8" s="55"/>
-      <c r="CX8" s="55"/>
-      <c r="CY8" s="55"/>
-      <c r="CZ8" s="55"/>
-      <c r="DA8" s="55"/>
-      <c r="DB8" s="55"/>
-      <c r="DC8" s="55"/>
-      <c r="DD8" s="55"/>
-      <c r="DE8" s="55"/>
-      <c r="DF8" s="55"/>
-      <c r="DG8" s="55"/>
-      <c r="DH8" s="55"/>
-      <c r="DI8" s="55"/>
-      <c r="DJ8" s="55"/>
-      <c r="DK8" s="55"/>
-      <c r="DL8" s="55"/>
-      <c r="DM8" s="55"/>
-      <c r="DN8" s="55"/>
-      <c r="DO8" s="55"/>
-      <c r="DP8" s="55"/>
-      <c r="DQ8" s="55"/>
-      <c r="DR8" s="55"/>
-      <c r="DS8" s="55"/>
-      <c r="DT8" s="55"/>
-      <c r="DU8" s="55"/>
-      <c r="DV8" s="55"/>
-      <c r="DW8" s="55"/>
-      <c r="DX8" s="55"/>
-      <c r="DY8" s="55"/>
-      <c r="DZ8" s="55"/>
-      <c r="EA8" s="55"/>
+      <c r="BL9" s="56"/>
+      <c r="BM9" s="56"/>
+      <c r="BN9" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO9" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="BP9" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="BQ9" s="55" t="n">
+        <v>7</v>
+      </c>
+      <c r="BR9" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="BS9" s="56"/>
+      <c r="BT9" s="56"/>
+      <c r="BU9" s="56"/>
+      <c r="BV9" s="56"/>
+      <c r="BW9" s="56"/>
+      <c r="BX9" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BY9" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BZ9" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="CA9" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="CB9" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC9" s="55" t="n">
+        <v>90.44</v>
+      </c>
+      <c r="CD9" s="55" t="n">
+        <v>140.67</v>
+      </c>
+      <c r="CE9" s="55" t="n">
+        <v>5.34</v>
+      </c>
+      <c r="CF9" s="55" t="n">
+        <v>43</v>
+      </c>
+      <c r="CG9" s="55" t="n">
+        <v>279.45</v>
+      </c>
+      <c r="CH9" s="56"/>
+      <c r="CI9" s="56"/>
+      <c r="CJ9" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="CK9" s="56"/>
+      <c r="CL9" s="55" t="n">
+        <v>14</v>
+      </c>
+      <c r="CM9" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="CN9" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="CO9" s="56"/>
+      <c r="CP9" s="56"/>
+      <c r="CQ9" s="56"/>
+      <c r="CR9" s="56"/>
+      <c r="CS9" s="55" t="n">
+        <v>29</v>
+      </c>
+      <c r="CT9" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="CU9" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="CV9" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW9" s="57" t="s">
+        <v>294</v>
+      </c>
+      <c r="CX9" s="56"/>
+      <c r="CY9" s="56"/>
+      <c r="CZ9" s="56"/>
+      <c r="DA9" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="DB9" s="56"/>
+      <c r="DC9" s="55" t="n">
+        <v>12</v>
+      </c>
+      <c r="DD9" s="56"/>
+      <c r="DE9" s="56"/>
+      <c r="DF9" s="56"/>
+      <c r="DG9" s="56"/>
+      <c r="DH9" s="55" t="n">
+        <v>107242</v>
+      </c>
+      <c r="DI9" s="57" t="s">
+        <v>289</v>
+      </c>
+      <c r="DJ9" s="55" t="n">
+        <v>107242</v>
+      </c>
+      <c r="DK9" s="56"/>
+      <c r="DL9" s="57" t="s">
+        <v>294</v>
+      </c>
+      <c r="DM9" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DN9" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DO9" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DP9" s="56"/>
+      <c r="DQ9" s="56"/>
+      <c r="DR9" s="56"/>
+      <c r="DS9" s="56"/>
+      <c r="DT9" s="56"/>
+      <c r="DU9" s="56"/>
+      <c r="DV9" s="56"/>
+      <c r="DW9" s="56"/>
+      <c r="DX9" s="56"/>
+      <c r="DY9" s="56"/>
+      <c r="DZ9" s="56"/>
+      <c r="EA9" s="56"/>
+      <c r="EB9" s="56"/>
+      <c r="EC9" s="56"/>
+      <c r="ED9" s="56"/>
+      <c r="EE9" s="56"/>
+      <c r="EF9" s="56"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="55"/>
-      <c r="R9" s="55"/>
-      <c r="S9" s="55"/>
-      <c r="T9" s="55"/>
-      <c r="U9" s="55"/>
-      <c r="V9" s="55"/>
-      <c r="W9" s="55"/>
-      <c r="X9" s="55"/>
-      <c r="Y9" s="55"/>
-      <c r="Z9" s="55"/>
-      <c r="AA9" s="55"/>
-      <c r="AB9" s="55"/>
-      <c r="AC9" s="55"/>
-      <c r="AD9" s="55"/>
-      <c r="AE9" s="55"/>
-      <c r="AF9" s="55"/>
-      <c r="AG9" s="55"/>
-      <c r="AH9" s="55"/>
-      <c r="AI9" s="55"/>
-      <c r="AJ9" s="55"/>
-      <c r="AK9" s="55"/>
-      <c r="AL9" s="55"/>
-      <c r="AM9" s="55"/>
-      <c r="AN9" s="55"/>
-      <c r="AO9" s="55"/>
-      <c r="AP9" s="55"/>
-      <c r="AQ9" s="55"/>
-      <c r="AR9" s="55"/>
-      <c r="AS9" s="55"/>
-      <c r="AT9" s="55"/>
-      <c r="AU9" s="55"/>
-      <c r="AV9" s="55"/>
-      <c r="AW9" s="55"/>
-      <c r="AX9" s="55"/>
-      <c r="AY9" s="55"/>
-      <c r="AZ9" s="55"/>
-      <c r="BA9" s="55"/>
-      <c r="BB9" s="55"/>
-      <c r="BC9" s="55"/>
-      <c r="BD9" s="55"/>
-      <c r="BE9" s="55"/>
-      <c r="BF9" s="55"/>
-      <c r="BG9" s="55"/>
-      <c r="BH9" s="55"/>
-      <c r="BI9" s="55"/>
-      <c r="BJ9" s="55"/>
-      <c r="BK9" s="55"/>
-      <c r="BL9" s="55"/>
-      <c r="BM9" s="55"/>
-      <c r="BN9" s="55"/>
-      <c r="BO9" s="55"/>
-      <c r="BP9" s="55"/>
-      <c r="BQ9" s="55"/>
-      <c r="BR9" s="55"/>
-      <c r="BS9" s="55"/>
-      <c r="BT9" s="55"/>
-      <c r="BU9" s="55"/>
-      <c r="BV9" s="55"/>
-      <c r="BW9" s="55"/>
-      <c r="BX9" s="55"/>
-      <c r="BY9" s="55"/>
-      <c r="BZ9" s="55"/>
-      <c r="CA9" s="55"/>
-      <c r="CB9" s="55"/>
-      <c r="CC9" s="55"/>
-      <c r="CD9" s="55"/>
-      <c r="CE9" s="55"/>
-      <c r="CF9" s="55"/>
-      <c r="CG9" s="55"/>
-      <c r="CH9" s="55"/>
-      <c r="CI9" s="55"/>
-      <c r="CJ9" s="55"/>
-      <c r="CK9" s="55"/>
-      <c r="CL9" s="55"/>
-      <c r="CM9" s="55"/>
-      <c r="CN9" s="55"/>
-      <c r="CO9" s="55"/>
-      <c r="CP9" s="55"/>
-      <c r="CQ9" s="55"/>
-      <c r="CR9" s="55"/>
-      <c r="CS9" s="55"/>
-      <c r="CT9" s="55"/>
-      <c r="CU9" s="55"/>
-      <c r="CV9" s="55"/>
-      <c r="CW9" s="55"/>
-      <c r="CX9" s="55"/>
-      <c r="CY9" s="55"/>
-      <c r="CZ9" s="55"/>
-      <c r="DA9" s="55"/>
-      <c r="DB9" s="55"/>
-      <c r="DC9" s="55"/>
-      <c r="DD9" s="55"/>
-      <c r="DE9" s="55"/>
-      <c r="DF9" s="55"/>
-      <c r="DG9" s="55"/>
-      <c r="DH9" s="55"/>
-      <c r="DI9" s="55"/>
-      <c r="DJ9" s="55"/>
-      <c r="DK9" s="55"/>
-      <c r="DL9" s="55"/>
-      <c r="DM9" s="55"/>
-      <c r="DN9" s="55"/>
-      <c r="DO9" s="55"/>
-      <c r="DP9" s="55"/>
-      <c r="DQ9" s="55"/>
-      <c r="DR9" s="55"/>
-      <c r="DS9" s="55"/>
-      <c r="DT9" s="55"/>
-      <c r="DU9" s="55"/>
-      <c r="DV9" s="55"/>
-      <c r="DW9" s="55"/>
-      <c r="DX9" s="55"/>
-      <c r="DY9" s="55"/>
-      <c r="DZ9" s="55"/>
-      <c r="EA9" s="56"/>
+    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="56"/>
+      <c r="H10" s="55" t="n">
+        <v>4198</v>
+      </c>
+      <c r="I10" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" s="55" t="n">
+        <v>5</v>
+      </c>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="55" t="n">
+        <v>41</v>
+      </c>
+      <c r="N10" s="56"/>
+      <c r="O10" s="56"/>
+      <c r="P10" s="56"/>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="56"/>
+      <c r="S10" s="56"/>
+      <c r="T10" s="56"/>
+      <c r="U10" s="57" t="s">
+        <v>286</v>
+      </c>
+      <c r="V10" s="56"/>
+      <c r="W10" s="56"/>
+      <c r="X10" s="56"/>
+      <c r="Y10" s="56"/>
+      <c r="Z10" s="56"/>
+      <c r="AA10" s="56"/>
+      <c r="AB10" s="56"/>
+      <c r="AC10" s="56"/>
+      <c r="AD10" s="56"/>
+      <c r="AE10" s="56"/>
+      <c r="AF10" s="56"/>
+      <c r="AG10" s="56"/>
+      <c r="AH10" s="56"/>
+      <c r="AI10" s="56"/>
+      <c r="AJ10" s="55" t="n">
+        <v>8</v>
+      </c>
+      <c r="AK10" s="56"/>
+      <c r="AL10" s="56"/>
+      <c r="AM10" s="56"/>
+      <c r="AN10" s="56"/>
+      <c r="AO10" s="56"/>
+      <c r="AP10" s="56"/>
+      <c r="AQ10" s="56"/>
+      <c r="AR10" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS10" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT10" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU10" s="56"/>
+      <c r="AV10" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW10" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AX10" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AY10" s="56"/>
+      <c r="AZ10" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA10" s="55" t="n">
+        <v>28</v>
+      </c>
+      <c r="BB10" s="56"/>
+      <c r="BC10" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="BD10" s="56"/>
+      <c r="BE10" s="56"/>
+      <c r="BF10" s="56"/>
+      <c r="BG10" s="56"/>
+      <c r="BH10" s="56"/>
+      <c r="BI10" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ10" s="55" t="n">
+        <v>28</v>
+      </c>
+      <c r="BK10" s="57" t="s">
+        <v>287</v>
+      </c>
+      <c r="BL10" s="56"/>
+      <c r="BM10" s="56"/>
+      <c r="BN10" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO10" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="BP10" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="BQ10" s="55" t="n">
+        <v>7</v>
+      </c>
+      <c r="BR10" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="BS10" s="56"/>
+      <c r="BT10" s="56"/>
+      <c r="BU10" s="56"/>
+      <c r="BV10" s="56"/>
+      <c r="BW10" s="56"/>
+      <c r="BX10" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BY10" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BZ10" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="CA10" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="CB10" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC10" s="55" t="n">
+        <v>90.44</v>
+      </c>
+      <c r="CD10" s="55" t="n">
+        <v>140.67</v>
+      </c>
+      <c r="CE10" s="55" t="n">
+        <v>5.34</v>
+      </c>
+      <c r="CF10" s="55" t="n">
+        <v>43</v>
+      </c>
+      <c r="CG10" s="55" t="n">
+        <v>279.45</v>
+      </c>
+      <c r="CH10" s="56"/>
+      <c r="CI10" s="56"/>
+      <c r="CJ10" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="CK10" s="56"/>
+      <c r="CL10" s="55" t="n">
+        <v>26</v>
+      </c>
+      <c r="CM10" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="CN10" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="CO10" s="56"/>
+      <c r="CP10" s="56"/>
+      <c r="CQ10" s="56"/>
+      <c r="CR10" s="56"/>
+      <c r="CS10" s="55" t="n">
+        <v>30</v>
+      </c>
+      <c r="CT10" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="CU10" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="CV10" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW10" s="57" t="s">
+        <v>295</v>
+      </c>
+      <c r="CX10" s="56"/>
+      <c r="CY10" s="56"/>
+      <c r="CZ10" s="56"/>
+      <c r="DA10" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="DB10" s="56"/>
+      <c r="DC10" s="55" t="n">
+        <v>12</v>
+      </c>
+      <c r="DD10" s="56"/>
+      <c r="DE10" s="56"/>
+      <c r="DF10" s="56"/>
+      <c r="DG10" s="56"/>
+      <c r="DH10" s="55" t="n">
+        <v>107242</v>
+      </c>
+      <c r="DI10" s="57" t="s">
+        <v>289</v>
+      </c>
+      <c r="DJ10" s="55" t="n">
+        <v>107242</v>
+      </c>
+      <c r="DK10" s="56"/>
+      <c r="DL10" s="57" t="s">
+        <v>295</v>
+      </c>
+      <c r="DM10" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DN10" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DO10" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DP10" s="56"/>
+      <c r="DQ10" s="56"/>
+      <c r="DR10" s="56"/>
+      <c r="DS10" s="56"/>
+      <c r="DT10" s="56"/>
+      <c r="DU10" s="56"/>
+      <c r="DV10" s="56"/>
+      <c r="DW10" s="56"/>
+      <c r="DX10" s="56"/>
+      <c r="DY10" s="56"/>
+      <c r="DZ10" s="56"/>
+      <c r="EA10" s="56"/>
+      <c r="EB10" s="56"/>
+      <c r="EC10" s="56"/>
+      <c r="ED10" s="56"/>
+      <c r="EE10" s="56"/>
+      <c r="EF10" s="56"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="55"/>
-      <c r="N10" s="55"/>
-      <c r="O10" s="55"/>
-      <c r="P10" s="55"/>
-      <c r="Q10" s="55"/>
-      <c r="R10" s="55"/>
-      <c r="S10" s="55"/>
-      <c r="T10" s="55"/>
-      <c r="U10" s="55"/>
-      <c r="V10" s="55"/>
-      <c r="W10" s="55"/>
-      <c r="X10" s="55"/>
-      <c r="Y10" s="55"/>
-      <c r="Z10" s="55"/>
-      <c r="AA10" s="55"/>
-      <c r="AB10" s="55"/>
-      <c r="AC10" s="55"/>
-      <c r="AD10" s="55"/>
-      <c r="AE10" s="55"/>
-      <c r="AF10" s="55"/>
-      <c r="AG10" s="55"/>
-      <c r="AH10" s="55"/>
-      <c r="AI10" s="55"/>
-      <c r="AJ10" s="55"/>
-      <c r="AK10" s="55"/>
-      <c r="AL10" s="55"/>
-      <c r="AM10" s="55"/>
-      <c r="AN10" s="55"/>
-      <c r="AO10" s="55"/>
-      <c r="AP10" s="55"/>
-      <c r="AQ10" s="55"/>
-      <c r="AR10" s="55"/>
-      <c r="AS10" s="55"/>
-      <c r="AT10" s="55"/>
-      <c r="AU10" s="55"/>
-      <c r="AV10" s="55"/>
-      <c r="AW10" s="55"/>
-      <c r="AX10" s="55"/>
-      <c r="AY10" s="55"/>
-      <c r="AZ10" s="55"/>
-      <c r="BA10" s="55"/>
-      <c r="BB10" s="55"/>
-      <c r="BC10" s="55"/>
-      <c r="BD10" s="55"/>
-      <c r="BE10" s="55"/>
-      <c r="BF10" s="55"/>
-      <c r="BG10" s="55"/>
-      <c r="BH10" s="55"/>
-      <c r="BI10" s="55"/>
-      <c r="BJ10" s="55"/>
-      <c r="BK10" s="55"/>
-      <c r="BL10" s="55"/>
-      <c r="BM10" s="55"/>
-      <c r="BN10" s="55"/>
-      <c r="BO10" s="55"/>
-      <c r="BP10" s="55"/>
-      <c r="BQ10" s="55"/>
-      <c r="BR10" s="55"/>
-      <c r="BS10" s="55"/>
-      <c r="BT10" s="55"/>
-      <c r="BU10" s="55"/>
-      <c r="BV10" s="55"/>
-      <c r="BW10" s="55"/>
-      <c r="BX10" s="55"/>
-      <c r="BY10" s="55"/>
-      <c r="BZ10" s="55"/>
-      <c r="CA10" s="55"/>
-      <c r="CB10" s="55"/>
-      <c r="CC10" s="55"/>
-      <c r="CD10" s="55"/>
-      <c r="CE10" s="55"/>
-      <c r="CF10" s="55"/>
-      <c r="CG10" s="55"/>
-      <c r="CH10" s="55"/>
-      <c r="CI10" s="55"/>
-      <c r="CJ10" s="55"/>
-      <c r="CK10" s="55"/>
-      <c r="CL10" s="55"/>
-      <c r="CM10" s="55"/>
-      <c r="CN10" s="55"/>
-      <c r="CO10" s="55"/>
-      <c r="CP10" s="55"/>
-      <c r="CQ10" s="55"/>
-      <c r="CR10" s="55"/>
-      <c r="CS10" s="55"/>
-      <c r="CT10" s="55"/>
-      <c r="CU10" s="55"/>
-      <c r="CV10" s="55"/>
-      <c r="CW10" s="55"/>
-      <c r="CX10" s="55"/>
-      <c r="CY10" s="55"/>
-      <c r="CZ10" s="55"/>
-      <c r="DA10" s="55"/>
-      <c r="DB10" s="55"/>
-      <c r="DC10" s="55"/>
-      <c r="DD10" s="55"/>
-      <c r="DE10" s="55"/>
-      <c r="DF10" s="55"/>
-      <c r="DG10" s="55"/>
-      <c r="DH10" s="55"/>
-      <c r="DI10" s="55"/>
-      <c r="DJ10" s="55"/>
-      <c r="DK10" s="55"/>
-      <c r="DL10" s="55"/>
-      <c r="DM10" s="55"/>
-      <c r="DN10" s="55"/>
-      <c r="DO10" s="55"/>
-      <c r="DP10" s="55"/>
-      <c r="DQ10" s="55"/>
-      <c r="DR10" s="55"/>
-      <c r="DS10" s="55"/>
-      <c r="DT10" s="55"/>
-      <c r="DU10" s="55"/>
-      <c r="DV10" s="55"/>
-      <c r="DW10" s="55"/>
-      <c r="DX10" s="55"/>
-      <c r="DY10" s="55"/>
-      <c r="DZ10" s="55"/>
-      <c r="EA10" s="55"/>
+    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="56"/>
+      <c r="H11" s="55" t="n">
+        <v>4220</v>
+      </c>
+      <c r="I11" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" s="55" t="n">
+        <v>5</v>
+      </c>
+      <c r="K11" s="56"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="57" t="s">
+        <v>290</v>
+      </c>
+      <c r="N11" s="56"/>
+      <c r="O11" s="56"/>
+      <c r="P11" s="56"/>
+      <c r="Q11" s="56"/>
+      <c r="R11" s="56"/>
+      <c r="S11" s="56"/>
+      <c r="T11" s="56"/>
+      <c r="U11" s="57" t="s">
+        <v>290</v>
+      </c>
+      <c r="V11" s="56"/>
+      <c r="W11" s="56"/>
+      <c r="X11" s="56"/>
+      <c r="Y11" s="56"/>
+      <c r="Z11" s="56"/>
+      <c r="AA11" s="56"/>
+      <c r="AB11" s="56"/>
+      <c r="AC11" s="56"/>
+      <c r="AD11" s="56"/>
+      <c r="AE11" s="56"/>
+      <c r="AF11" s="56"/>
+      <c r="AG11" s="56"/>
+      <c r="AH11" s="56"/>
+      <c r="AI11" s="56"/>
+      <c r="AJ11" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="56"/>
+      <c r="AL11" s="56"/>
+      <c r="AM11" s="56"/>
+      <c r="AN11" s="56"/>
+      <c r="AO11" s="56"/>
+      <c r="AP11" s="56"/>
+      <c r="AQ11" s="56"/>
+      <c r="AR11" s="55" t="n">
+        <v>17</v>
+      </c>
+      <c r="AS11" s="55" t="n">
+        <v>13</v>
+      </c>
+      <c r="AT11" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU11" s="56"/>
+      <c r="AV11" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW11" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AX11" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AY11" s="56"/>
+      <c r="AZ11" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA11" s="55" t="n">
+        <v>28</v>
+      </c>
+      <c r="BB11" s="56"/>
+      <c r="BC11" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="BD11" s="56"/>
+      <c r="BE11" s="56"/>
+      <c r="BF11" s="56"/>
+      <c r="BG11" s="56"/>
+      <c r="BH11" s="56"/>
+      <c r="BI11" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ11" s="55" t="n">
+        <v>25</v>
+      </c>
+      <c r="BK11" s="57" t="s">
+        <v>291</v>
+      </c>
+      <c r="BL11" s="56"/>
+      <c r="BM11" s="56"/>
+      <c r="BN11" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO11" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="BP11" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="BQ11" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR11" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="BS11" s="56"/>
+      <c r="BT11" s="56"/>
+      <c r="BU11" s="56"/>
+      <c r="BV11" s="56"/>
+      <c r="BW11" s="56"/>
+      <c r="BX11" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BY11" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BZ11" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="CA11" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="CB11" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC11" s="55" t="n">
+        <v>90.44</v>
+      </c>
+      <c r="CD11" s="55" t="n">
+        <v>140.67</v>
+      </c>
+      <c r="CE11" s="55" t="n">
+        <v>5.34</v>
+      </c>
+      <c r="CF11" s="55" t="n">
+        <v>43</v>
+      </c>
+      <c r="CG11" s="55" t="n">
+        <v>279.45</v>
+      </c>
+      <c r="CH11" s="56"/>
+      <c r="CI11" s="56"/>
+      <c r="CJ11" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="CK11" s="56"/>
+      <c r="CL11" s="55" t="n">
+        <v>13</v>
+      </c>
+      <c r="CM11" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="CN11" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="CO11" s="56"/>
+      <c r="CP11" s="56"/>
+      <c r="CQ11" s="56"/>
+      <c r="CR11" s="56"/>
+      <c r="CS11" s="55" t="n">
+        <v>8</v>
+      </c>
+      <c r="CT11" s="55" t="n">
+        <v>5</v>
+      </c>
+      <c r="CU11" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="CV11" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW11" s="57" t="s">
+        <v>296</v>
+      </c>
+      <c r="CX11" s="56"/>
+      <c r="CY11" s="56"/>
+      <c r="CZ11" s="56"/>
+      <c r="DA11" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="DB11" s="56"/>
+      <c r="DC11" s="55" t="n">
+        <v>12</v>
+      </c>
+      <c r="DD11" s="56"/>
+      <c r="DE11" s="56"/>
+      <c r="DF11" s="56"/>
+      <c r="DG11" s="56"/>
+      <c r="DH11" s="55" t="n">
+        <v>107242</v>
+      </c>
+      <c r="DI11" s="57" t="s">
+        <v>289</v>
+      </c>
+      <c r="DJ11" s="55" t="n">
+        <v>107242</v>
+      </c>
+      <c r="DK11" s="56"/>
+      <c r="DL11" s="57" t="s">
+        <v>296</v>
+      </c>
+      <c r="DM11" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DN11" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DO11" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DP11" s="56"/>
+      <c r="DQ11" s="56"/>
+      <c r="DR11" s="56"/>
+      <c r="DS11" s="56"/>
+      <c r="DT11" s="56"/>
+      <c r="DU11" s="56"/>
+      <c r="DV11" s="56"/>
+      <c r="DW11" s="56"/>
+      <c r="DX11" s="56"/>
+      <c r="DY11" s="56"/>
+      <c r="DZ11" s="56"/>
+      <c r="EA11" s="56"/>
+      <c r="EB11" s="56"/>
+      <c r="EC11" s="56"/>
+      <c r="ED11" s="56"/>
+      <c r="EE11" s="56"/>
+      <c r="EF11" s="56"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="55"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="55"/>
-      <c r="M11" s="55"/>
-      <c r="N11" s="55"/>
-      <c r="O11" s="55"/>
-      <c r="P11" s="55"/>
-      <c r="Q11" s="55"/>
-      <c r="R11" s="55"/>
-      <c r="S11" s="55"/>
-      <c r="T11" s="55"/>
-      <c r="U11" s="55"/>
-      <c r="V11" s="55"/>
-      <c r="W11" s="55"/>
-      <c r="X11" s="55"/>
-      <c r="Y11" s="55"/>
-      <c r="Z11" s="55"/>
-      <c r="AA11" s="55"/>
-      <c r="AB11" s="55"/>
-      <c r="AC11" s="55"/>
-      <c r="AD11" s="55"/>
-      <c r="AE11" s="55"/>
-      <c r="AF11" s="55"/>
-      <c r="AG11" s="55"/>
-      <c r="AH11" s="55"/>
-      <c r="AI11" s="55"/>
-      <c r="AJ11" s="55"/>
-      <c r="AK11" s="55"/>
-      <c r="AL11" s="55"/>
-      <c r="AM11" s="55"/>
-      <c r="AN11" s="55"/>
-      <c r="AO11" s="55"/>
-      <c r="AP11" s="55"/>
-      <c r="AQ11" s="55"/>
-      <c r="AR11" s="55"/>
-      <c r="AS11" s="55"/>
-      <c r="AT11" s="55"/>
-      <c r="AU11" s="55"/>
-      <c r="AV11" s="55"/>
-      <c r="AW11" s="55"/>
-      <c r="AX11" s="55"/>
-      <c r="AY11" s="55"/>
-      <c r="AZ11" s="55"/>
-      <c r="BA11" s="55"/>
-      <c r="BB11" s="55"/>
-      <c r="BC11" s="55"/>
-      <c r="BD11" s="55"/>
-      <c r="BE11" s="55"/>
-      <c r="BF11" s="55"/>
-      <c r="BG11" s="55"/>
-      <c r="BH11" s="55"/>
-      <c r="BI11" s="55"/>
-      <c r="BJ11" s="55"/>
-      <c r="BK11" s="55"/>
-      <c r="BL11" s="55"/>
-      <c r="BM11" s="55"/>
-      <c r="BN11" s="55"/>
-      <c r="BO11" s="55"/>
-      <c r="BP11" s="55"/>
-      <c r="BQ11" s="55"/>
-      <c r="BR11" s="55"/>
-      <c r="BS11" s="55"/>
-      <c r="BT11" s="55"/>
-      <c r="BU11" s="55"/>
-      <c r="BV11" s="55"/>
-      <c r="BW11" s="55"/>
-      <c r="BX11" s="55"/>
-      <c r="BY11" s="55"/>
-      <c r="BZ11" s="55"/>
-      <c r="CA11" s="55"/>
-      <c r="CB11" s="55"/>
-      <c r="CC11" s="55"/>
-      <c r="CD11" s="55"/>
-      <c r="CE11" s="55"/>
-      <c r="CF11" s="55"/>
-      <c r="CG11" s="55"/>
-      <c r="CH11" s="55"/>
-      <c r="CI11" s="55"/>
-      <c r="CJ11" s="55"/>
-      <c r="CK11" s="55"/>
-      <c r="CL11" s="55"/>
-      <c r="CM11" s="55"/>
-      <c r="CN11" s="55"/>
-      <c r="CO11" s="55"/>
-      <c r="CP11" s="55"/>
-      <c r="CQ11" s="55"/>
-      <c r="CR11" s="55"/>
-      <c r="CS11" s="55"/>
-      <c r="CT11" s="55"/>
-      <c r="CU11" s="55"/>
-      <c r="CV11" s="55"/>
-      <c r="CW11" s="55"/>
-      <c r="CX11" s="55"/>
-      <c r="CY11" s="55"/>
-      <c r="CZ11" s="55"/>
-      <c r="DA11" s="55"/>
-      <c r="DB11" s="55"/>
-      <c r="DC11" s="55"/>
-      <c r="DD11" s="55"/>
-      <c r="DE11" s="55"/>
-      <c r="DF11" s="55"/>
-      <c r="DG11" s="55"/>
-      <c r="DH11" s="55"/>
-      <c r="DI11" s="55"/>
-      <c r="DJ11" s="55"/>
-      <c r="DK11" s="55"/>
-      <c r="DL11" s="55"/>
-      <c r="DM11" s="55"/>
-      <c r="DN11" s="55"/>
-      <c r="DO11" s="55"/>
-      <c r="DP11" s="55"/>
-      <c r="DQ11" s="55"/>
-      <c r="DR11" s="55"/>
-      <c r="DS11" s="55"/>
-      <c r="DT11" s="55"/>
-      <c r="DU11" s="55"/>
-      <c r="DV11" s="55"/>
-      <c r="DW11" s="55"/>
-      <c r="DX11" s="55"/>
-      <c r="DY11" s="55"/>
-      <c r="DZ11" s="55"/>
-      <c r="EA11" s="55"/>
+    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="56"/>
+      <c r="H12" s="55" t="n">
+        <v>4285</v>
+      </c>
+      <c r="I12" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" s="55" t="n">
+        <v>5</v>
+      </c>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="57" t="s">
+        <v>290</v>
+      </c>
+      <c r="N12" s="56"/>
+      <c r="O12" s="56"/>
+      <c r="P12" s="56"/>
+      <c r="Q12" s="56"/>
+      <c r="R12" s="56"/>
+      <c r="S12" s="56"/>
+      <c r="T12" s="56"/>
+      <c r="U12" s="57" t="s">
+        <v>290</v>
+      </c>
+      <c r="V12" s="56"/>
+      <c r="W12" s="56"/>
+      <c r="X12" s="56"/>
+      <c r="Y12" s="56"/>
+      <c r="Z12" s="56"/>
+      <c r="AA12" s="56"/>
+      <c r="AB12" s="56"/>
+      <c r="AC12" s="56"/>
+      <c r="AD12" s="56"/>
+      <c r="AE12" s="56"/>
+      <c r="AF12" s="56"/>
+      <c r="AG12" s="56"/>
+      <c r="AH12" s="56"/>
+      <c r="AI12" s="56"/>
+      <c r="AJ12" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="56"/>
+      <c r="AL12" s="56"/>
+      <c r="AM12" s="56"/>
+      <c r="AN12" s="56"/>
+      <c r="AO12" s="56"/>
+      <c r="AP12" s="56"/>
+      <c r="AQ12" s="56"/>
+      <c r="AR12" s="55" t="n">
+        <v>17</v>
+      </c>
+      <c r="AS12" s="55" t="n">
+        <v>13</v>
+      </c>
+      <c r="AT12" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU12" s="56"/>
+      <c r="AV12" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW12" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AX12" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AY12" s="56"/>
+      <c r="AZ12" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA12" s="55" t="n">
+        <v>28</v>
+      </c>
+      <c r="BB12" s="56"/>
+      <c r="BC12" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="BD12" s="56"/>
+      <c r="BE12" s="56"/>
+      <c r="BF12" s="56"/>
+      <c r="BG12" s="56"/>
+      <c r="BH12" s="56"/>
+      <c r="BI12" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ12" s="55" t="n">
+        <v>25</v>
+      </c>
+      <c r="BK12" s="57" t="s">
+        <v>291</v>
+      </c>
+      <c r="BL12" s="56"/>
+      <c r="BM12" s="56"/>
+      <c r="BN12" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO12" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="BP12" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="BQ12" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR12" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="BS12" s="56"/>
+      <c r="BT12" s="56"/>
+      <c r="BU12" s="56"/>
+      <c r="BV12" s="56"/>
+      <c r="BW12" s="56"/>
+      <c r="BX12" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BY12" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BZ12" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="CA12" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="CB12" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC12" s="55" t="n">
+        <v>90.44</v>
+      </c>
+      <c r="CD12" s="55" t="n">
+        <v>140.67</v>
+      </c>
+      <c r="CE12" s="55" t="n">
+        <v>5.34</v>
+      </c>
+      <c r="CF12" s="55" t="n">
+        <v>43</v>
+      </c>
+      <c r="CG12" s="55" t="n">
+        <v>279.45</v>
+      </c>
+      <c r="CH12" s="56"/>
+      <c r="CI12" s="56"/>
+      <c r="CJ12" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="CK12" s="56"/>
+      <c r="CL12" s="55" t="n">
+        <v>7</v>
+      </c>
+      <c r="CM12" s="55" t="n">
+        <v>5</v>
+      </c>
+      <c r="CN12" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="CO12" s="56"/>
+      <c r="CP12" s="56"/>
+      <c r="CQ12" s="56"/>
+      <c r="CR12" s="56"/>
+      <c r="CS12" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="CT12" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="CU12" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="CV12" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW12" s="57" t="s">
+        <v>297</v>
+      </c>
+      <c r="CX12" s="56"/>
+      <c r="CY12" s="56"/>
+      <c r="CZ12" s="56"/>
+      <c r="DA12" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="DB12" s="56"/>
+      <c r="DC12" s="55" t="n">
+        <v>8</v>
+      </c>
+      <c r="DD12" s="56"/>
+      <c r="DE12" s="56"/>
+      <c r="DF12" s="56"/>
+      <c r="DG12" s="56"/>
+      <c r="DH12" s="55" t="n">
+        <v>107242</v>
+      </c>
+      <c r="DI12" s="57" t="s">
+        <v>289</v>
+      </c>
+      <c r="DJ12" s="55" t="n">
+        <v>107242</v>
+      </c>
+      <c r="DK12" s="56"/>
+      <c r="DL12" s="57" t="s">
+        <v>297</v>
+      </c>
+      <c r="DM12" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DN12" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DO12" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DP12" s="56"/>
+      <c r="DQ12" s="56"/>
+      <c r="DR12" s="56"/>
+      <c r="DS12" s="56"/>
+      <c r="DT12" s="56"/>
+      <c r="DU12" s="56"/>
+      <c r="DV12" s="56"/>
+      <c r="DW12" s="56"/>
+      <c r="DX12" s="56"/>
+      <c r="DY12" s="56"/>
+      <c r="DZ12" s="56"/>
+      <c r="EA12" s="56"/>
+      <c r="EB12" s="56"/>
+      <c r="EC12" s="56"/>
+      <c r="ED12" s="56"/>
+      <c r="EE12" s="56"/>
+      <c r="EF12" s="56"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="55"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="55"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="55"/>
-      <c r="P12" s="55"/>
-      <c r="Q12" s="55"/>
-      <c r="R12" s="55"/>
-      <c r="S12" s="55"/>
-      <c r="T12" s="55"/>
-      <c r="U12" s="55"/>
-      <c r="V12" s="55"/>
-      <c r="W12" s="55"/>
-      <c r="X12" s="55"/>
-      <c r="Y12" s="55"/>
-      <c r="Z12" s="55"/>
-      <c r="AA12" s="55"/>
-      <c r="AB12" s="55"/>
-      <c r="AC12" s="55"/>
-      <c r="AD12" s="55"/>
-      <c r="AE12" s="55"/>
-      <c r="AF12" s="55"/>
-      <c r="AG12" s="55"/>
-      <c r="AH12" s="55"/>
-      <c r="AI12" s="55"/>
-      <c r="AJ12" s="55"/>
-      <c r="AK12" s="55"/>
-      <c r="AL12" s="55"/>
-      <c r="AM12" s="55"/>
-      <c r="AN12" s="55"/>
-      <c r="AO12" s="55"/>
-      <c r="AP12" s="55"/>
-      <c r="AQ12" s="55"/>
-      <c r="AR12" s="55"/>
-      <c r="AS12" s="55"/>
-      <c r="AT12" s="55"/>
-      <c r="AU12" s="55"/>
-      <c r="AV12" s="55"/>
-      <c r="AW12" s="55"/>
-      <c r="AX12" s="55"/>
-      <c r="AY12" s="55"/>
-      <c r="AZ12" s="55"/>
-      <c r="BA12" s="55"/>
-      <c r="BB12" s="55"/>
-      <c r="BC12" s="55"/>
-      <c r="BD12" s="55"/>
-      <c r="BE12" s="55"/>
-      <c r="BF12" s="55"/>
-      <c r="BG12" s="55"/>
-      <c r="BH12" s="55"/>
-      <c r="BI12" s="55"/>
-      <c r="BJ12" s="55"/>
-      <c r="BK12" s="55"/>
-      <c r="BL12" s="55"/>
-      <c r="BM12" s="55"/>
-      <c r="BN12" s="55"/>
-      <c r="BO12" s="55"/>
-      <c r="BP12" s="55"/>
-      <c r="BQ12" s="55"/>
-      <c r="BR12" s="55"/>
-      <c r="BS12" s="55"/>
-      <c r="BT12" s="55"/>
-      <c r="BU12" s="55"/>
-      <c r="BV12" s="55"/>
-      <c r="BW12" s="55"/>
-      <c r="BX12" s="55"/>
-      <c r="BY12" s="55"/>
-      <c r="BZ12" s="55"/>
-      <c r="CA12" s="55"/>
-      <c r="CB12" s="55"/>
-      <c r="CC12" s="55"/>
-      <c r="CD12" s="55"/>
-      <c r="CE12" s="55"/>
-      <c r="CF12" s="55"/>
-      <c r="CG12" s="55"/>
-      <c r="CH12" s="55"/>
-      <c r="CI12" s="55"/>
-      <c r="CJ12" s="55"/>
-      <c r="CK12" s="55"/>
-      <c r="CL12" s="55"/>
-      <c r="CM12" s="55"/>
-      <c r="CN12" s="55"/>
-      <c r="CO12" s="55"/>
-      <c r="CP12" s="55"/>
-      <c r="CQ12" s="55"/>
-      <c r="CR12" s="55"/>
-      <c r="CS12" s="55"/>
-      <c r="CT12" s="55"/>
-      <c r="CU12" s="55"/>
-      <c r="CV12" s="55"/>
-      <c r="CW12" s="55"/>
-      <c r="CX12" s="55"/>
-      <c r="CY12" s="55"/>
-      <c r="CZ12" s="55"/>
-      <c r="DA12" s="55"/>
-      <c r="DB12" s="55"/>
-      <c r="DC12" s="55"/>
-      <c r="DD12" s="55"/>
-      <c r="DE12" s="55"/>
-      <c r="DF12" s="55"/>
-      <c r="DG12" s="55"/>
-      <c r="DH12" s="55"/>
-      <c r="DI12" s="55"/>
-      <c r="DJ12" s="55"/>
-      <c r="DK12" s="55"/>
-      <c r="DL12" s="55"/>
-      <c r="DM12" s="55"/>
-      <c r="DN12" s="55"/>
-      <c r="DO12" s="55"/>
-      <c r="DP12" s="55"/>
-      <c r="DQ12" s="55"/>
-      <c r="DR12" s="55"/>
-      <c r="DS12" s="55"/>
-      <c r="DT12" s="55"/>
-      <c r="DU12" s="55"/>
-      <c r="DV12" s="55"/>
-      <c r="DW12" s="55"/>
-      <c r="DX12" s="55"/>
-      <c r="DY12" s="55"/>
-      <c r="DZ12" s="55"/>
-      <c r="EA12" s="55"/>
+    <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="56"/>
+      <c r="H13" s="55" t="n">
+        <v>4189</v>
+      </c>
+      <c r="I13" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="J13" s="55" t="n">
+        <v>5</v>
+      </c>
+      <c r="K13" s="56"/>
+      <c r="L13" s="56"/>
+      <c r="M13" s="55" t="n">
+        <v>27</v>
+      </c>
+      <c r="N13" s="56"/>
+      <c r="O13" s="56"/>
+      <c r="P13" s="56"/>
+      <c r="Q13" s="56"/>
+      <c r="R13" s="56"/>
+      <c r="S13" s="56"/>
+      <c r="T13" s="56"/>
+      <c r="U13" s="57" t="s">
+        <v>293</v>
+      </c>
+      <c r="V13" s="56"/>
+      <c r="W13" s="56"/>
+      <c r="X13" s="56"/>
+      <c r="Y13" s="56"/>
+      <c r="Z13" s="56"/>
+      <c r="AA13" s="56"/>
+      <c r="AB13" s="56"/>
+      <c r="AC13" s="56"/>
+      <c r="AD13" s="56"/>
+      <c r="AE13" s="56"/>
+      <c r="AF13" s="56"/>
+      <c r="AG13" s="56"/>
+      <c r="AH13" s="56"/>
+      <c r="AI13" s="56"/>
+      <c r="AJ13" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AK13" s="56"/>
+      <c r="AL13" s="56"/>
+      <c r="AM13" s="56"/>
+      <c r="AN13" s="56"/>
+      <c r="AO13" s="56"/>
+      <c r="AP13" s="56"/>
+      <c r="AQ13" s="56"/>
+      <c r="AR13" s="55" t="n">
+        <v>12</v>
+      </c>
+      <c r="AS13" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT13" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="AU13" s="56"/>
+      <c r="AV13" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW13" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX13" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AY13" s="56"/>
+      <c r="AZ13" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA13" s="55" t="n">
+        <v>18</v>
+      </c>
+      <c r="BB13" s="56"/>
+      <c r="BC13" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="BD13" s="56"/>
+      <c r="BE13" s="56"/>
+      <c r="BF13" s="56"/>
+      <c r="BG13" s="56"/>
+      <c r="BH13" s="56"/>
+      <c r="BI13" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ13" s="55" t="n">
+        <v>18</v>
+      </c>
+      <c r="BK13" s="57" t="s">
+        <v>287</v>
+      </c>
+      <c r="BL13" s="56"/>
+      <c r="BM13" s="56"/>
+      <c r="BN13" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO13" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="BP13" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="BQ13" s="55" t="n">
+        <v>7</v>
+      </c>
+      <c r="BR13" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BS13" s="56"/>
+      <c r="BT13" s="56"/>
+      <c r="BU13" s="56"/>
+      <c r="BV13" s="56"/>
+      <c r="BW13" s="56"/>
+      <c r="BX13" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BY13" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BZ13" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="CA13" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="CB13" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC13" s="55" t="n">
+        <v>90.44</v>
+      </c>
+      <c r="CD13" s="55" t="n">
+        <v>140.67</v>
+      </c>
+      <c r="CE13" s="55" t="n">
+        <v>5.34</v>
+      </c>
+      <c r="CF13" s="55" t="n">
+        <v>43</v>
+      </c>
+      <c r="CG13" s="55" t="n">
+        <v>279.45</v>
+      </c>
+      <c r="CH13" s="56"/>
+      <c r="CI13" s="56"/>
+      <c r="CJ13" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="CK13" s="56"/>
+      <c r="CL13" s="55" t="n">
+        <v>17</v>
+      </c>
+      <c r="CM13" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="CN13" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="CO13" s="56"/>
+      <c r="CP13" s="56"/>
+      <c r="CQ13" s="56"/>
+      <c r="CR13" s="56"/>
+      <c r="CS13" s="55" t="n">
+        <v>26</v>
+      </c>
+      <c r="CT13" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="CU13" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="CV13" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW13" s="57" t="s">
+        <v>298</v>
+      </c>
+      <c r="CX13" s="56"/>
+      <c r="CY13" s="56"/>
+      <c r="CZ13" s="56"/>
+      <c r="DA13" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="DB13" s="56"/>
+      <c r="DC13" s="55" t="n">
+        <v>11</v>
+      </c>
+      <c r="DD13" s="56"/>
+      <c r="DE13" s="56"/>
+      <c r="DF13" s="56"/>
+      <c r="DG13" s="56"/>
+      <c r="DH13" s="55" t="n">
+        <v>107242</v>
+      </c>
+      <c r="DI13" s="57" t="s">
+        <v>289</v>
+      </c>
+      <c r="DJ13" s="55" t="n">
+        <v>107242</v>
+      </c>
+      <c r="DK13" s="56"/>
+      <c r="DL13" s="57" t="s">
+        <v>298</v>
+      </c>
+      <c r="DM13" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DN13" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DO13" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DP13" s="56"/>
+      <c r="DQ13" s="56"/>
+      <c r="DR13" s="56"/>
+      <c r="DS13" s="56"/>
+      <c r="DT13" s="56"/>
+      <c r="DU13" s="56"/>
+      <c r="DV13" s="56"/>
+      <c r="DW13" s="56"/>
+      <c r="DX13" s="56"/>
+      <c r="DY13" s="56"/>
+      <c r="DZ13" s="56"/>
+      <c r="EA13" s="56"/>
+      <c r="EB13" s="56"/>
+      <c r="EC13" s="56"/>
+      <c r="ED13" s="56"/>
+      <c r="EE13" s="56"/>
+      <c r="EF13" s="56"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="55"/>
-      <c r="L13" s="55"/>
-      <c r="M13" s="55"/>
-      <c r="N13" s="55"/>
-      <c r="O13" s="55"/>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="55"/>
-      <c r="R13" s="55"/>
-      <c r="S13" s="55"/>
-      <c r="T13" s="55"/>
-      <c r="U13" s="55"/>
-      <c r="V13" s="55"/>
-      <c r="W13" s="55"/>
-      <c r="X13" s="55"/>
-      <c r="Y13" s="55"/>
-      <c r="Z13" s="55"/>
-      <c r="AA13" s="55"/>
-      <c r="AB13" s="55"/>
-      <c r="AC13" s="55"/>
-      <c r="AD13" s="55"/>
-      <c r="AE13" s="55"/>
-      <c r="AF13" s="55"/>
-      <c r="AG13" s="55"/>
-      <c r="AH13" s="55"/>
-      <c r="AI13" s="55"/>
-      <c r="AJ13" s="55"/>
-      <c r="AK13" s="55"/>
-      <c r="AL13" s="55"/>
-      <c r="AM13" s="55"/>
-      <c r="AN13" s="55"/>
-      <c r="AO13" s="55"/>
-      <c r="AP13" s="55"/>
-      <c r="AQ13" s="55"/>
-      <c r="AR13" s="55"/>
-      <c r="AS13" s="55"/>
-      <c r="AT13" s="55"/>
-      <c r="AU13" s="55"/>
-      <c r="AV13" s="55"/>
-      <c r="AW13" s="55"/>
-      <c r="AX13" s="55"/>
-      <c r="AY13" s="55"/>
-      <c r="AZ13" s="55"/>
-      <c r="BA13" s="55"/>
-      <c r="BB13" s="55"/>
-      <c r="BC13" s="55"/>
-      <c r="BD13" s="55"/>
-      <c r="BE13" s="55"/>
-      <c r="BF13" s="55"/>
-      <c r="BG13" s="55"/>
-      <c r="BH13" s="55"/>
-      <c r="BI13" s="55"/>
-      <c r="BJ13" s="55"/>
-      <c r="BK13" s="55"/>
-      <c r="BL13" s="55"/>
-      <c r="BM13" s="55"/>
-      <c r="BN13" s="55"/>
-      <c r="BO13" s="55"/>
-      <c r="BP13" s="55"/>
-      <c r="BQ13" s="55"/>
-      <c r="BR13" s="55"/>
-      <c r="BS13" s="55"/>
-      <c r="BT13" s="55"/>
-      <c r="BU13" s="55"/>
-      <c r="BV13" s="55"/>
-      <c r="BW13" s="55"/>
-      <c r="BX13" s="55"/>
-      <c r="BY13" s="55"/>
-      <c r="BZ13" s="55"/>
-      <c r="CA13" s="55"/>
-      <c r="CB13" s="55"/>
-      <c r="CC13" s="55"/>
-      <c r="CD13" s="55"/>
-      <c r="CE13" s="55"/>
-      <c r="CF13" s="55"/>
-      <c r="CG13" s="55"/>
-      <c r="CH13" s="55"/>
-      <c r="CI13" s="55"/>
-      <c r="CJ13" s="55"/>
-      <c r="CK13" s="55"/>
-      <c r="CL13" s="55"/>
-      <c r="CM13" s="55"/>
-      <c r="CN13" s="55"/>
-      <c r="CO13" s="55"/>
-      <c r="CP13" s="55"/>
-      <c r="CQ13" s="55"/>
-      <c r="CR13" s="55"/>
-      <c r="CS13" s="55"/>
-      <c r="CT13" s="55"/>
-      <c r="CU13" s="55"/>
-      <c r="CV13" s="55"/>
-      <c r="CW13" s="55"/>
-      <c r="CX13" s="55"/>
-      <c r="CY13" s="55"/>
-      <c r="CZ13" s="55"/>
-      <c r="DA13" s="55"/>
-      <c r="DB13" s="55"/>
-      <c r="DC13" s="55"/>
-      <c r="DD13" s="55"/>
-      <c r="DE13" s="55"/>
-      <c r="DF13" s="55"/>
-      <c r="DG13" s="55"/>
-      <c r="DH13" s="55"/>
-      <c r="DI13" s="55"/>
-      <c r="DJ13" s="55"/>
-      <c r="DK13" s="55"/>
-      <c r="DL13" s="55"/>
-      <c r="DM13" s="55"/>
-      <c r="DN13" s="55"/>
-      <c r="DO13" s="55"/>
-      <c r="DP13" s="55"/>
-      <c r="DQ13" s="55"/>
-      <c r="DR13" s="55"/>
-      <c r="DS13" s="55"/>
-      <c r="DT13" s="55"/>
-      <c r="DU13" s="55"/>
-      <c r="DV13" s="55"/>
-      <c r="DW13" s="55"/>
-      <c r="DX13" s="55"/>
-      <c r="DY13" s="55"/>
-      <c r="DZ13" s="55"/>
-      <c r="EA13" s="56"/>
+    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="56"/>
+      <c r="H14" s="55" t="n">
+        <v>4533</v>
+      </c>
+      <c r="I14" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" s="55" t="n">
+        <v>5</v>
+      </c>
+      <c r="K14" s="56"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="55" t="n">
+        <v>30</v>
+      </c>
+      <c r="N14" s="56"/>
+      <c r="O14" s="56"/>
+      <c r="P14" s="56"/>
+      <c r="Q14" s="56"/>
+      <c r="R14" s="56"/>
+      <c r="S14" s="56"/>
+      <c r="T14" s="56"/>
+      <c r="U14" s="57" t="s">
+        <v>293</v>
+      </c>
+      <c r="V14" s="56"/>
+      <c r="W14" s="56"/>
+      <c r="X14" s="56"/>
+      <c r="Y14" s="56"/>
+      <c r="Z14" s="56"/>
+      <c r="AA14" s="56"/>
+      <c r="AB14" s="56"/>
+      <c r="AC14" s="56"/>
+      <c r="AD14" s="56"/>
+      <c r="AE14" s="56"/>
+      <c r="AF14" s="56"/>
+      <c r="AG14" s="56"/>
+      <c r="AH14" s="56"/>
+      <c r="AI14" s="56"/>
+      <c r="AJ14" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AK14" s="56"/>
+      <c r="AL14" s="56"/>
+      <c r="AM14" s="56"/>
+      <c r="AN14" s="56"/>
+      <c r="AO14" s="56"/>
+      <c r="AP14" s="56"/>
+      <c r="AQ14" s="56"/>
+      <c r="AR14" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS14" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT14" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU14" s="56"/>
+      <c r="AV14" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW14" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX14" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AY14" s="56"/>
+      <c r="AZ14" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA14" s="55" t="n">
+        <v>7</v>
+      </c>
+      <c r="BB14" s="56"/>
+      <c r="BC14" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="BD14" s="56"/>
+      <c r="BE14" s="56"/>
+      <c r="BF14" s="56"/>
+      <c r="BG14" s="56"/>
+      <c r="BH14" s="56"/>
+      <c r="BI14" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ14" s="55" t="n">
+        <v>7</v>
+      </c>
+      <c r="BK14" s="57" t="s">
+        <v>287</v>
+      </c>
+      <c r="BL14" s="56"/>
+      <c r="BM14" s="56"/>
+      <c r="BN14" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO14" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="BP14" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="BQ14" s="55" t="n">
+        <v>7</v>
+      </c>
+      <c r="BR14" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BS14" s="56"/>
+      <c r="BT14" s="56"/>
+      <c r="BU14" s="56"/>
+      <c r="BV14" s="56"/>
+      <c r="BW14" s="56"/>
+      <c r="BX14" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BY14" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BZ14" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="CA14" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="CB14" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC14" s="55" t="n">
+        <v>90.44</v>
+      </c>
+      <c r="CD14" s="55" t="n">
+        <v>140.67</v>
+      </c>
+      <c r="CE14" s="55" t="n">
+        <v>5.34</v>
+      </c>
+      <c r="CF14" s="55" t="n">
+        <v>43</v>
+      </c>
+      <c r="CG14" s="55" t="n">
+        <v>279.45</v>
+      </c>
+      <c r="CH14" s="56"/>
+      <c r="CI14" s="56"/>
+      <c r="CJ14" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="CK14" s="56"/>
+      <c r="CL14" s="55" t="n">
+        <v>22</v>
+      </c>
+      <c r="CM14" s="55" t="n">
+        <v>7</v>
+      </c>
+      <c r="CN14" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="CO14" s="56"/>
+      <c r="CP14" s="56"/>
+      <c r="CQ14" s="56"/>
+      <c r="CR14" s="56"/>
+      <c r="CS14" s="55" t="n">
+        <v>14</v>
+      </c>
+      <c r="CT14" s="55" t="n">
+        <v>8</v>
+      </c>
+      <c r="CU14" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="CV14" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW14" s="57" t="s">
+        <v>299</v>
+      </c>
+      <c r="CX14" s="56"/>
+      <c r="CY14" s="56"/>
+      <c r="CZ14" s="56"/>
+      <c r="DA14" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="DB14" s="56"/>
+      <c r="DC14" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="DD14" s="56"/>
+      <c r="DE14" s="56"/>
+      <c r="DF14" s="56"/>
+      <c r="DG14" s="56"/>
+      <c r="DH14" s="55" t="n">
+        <v>107242</v>
+      </c>
+      <c r="DI14" s="57" t="s">
+        <v>289</v>
+      </c>
+      <c r="DJ14" s="55" t="n">
+        <v>107242</v>
+      </c>
+      <c r="DK14" s="56"/>
+      <c r="DL14" s="57" t="s">
+        <v>299</v>
+      </c>
+      <c r="DM14" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DN14" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DO14" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DP14" s="56"/>
+      <c r="DQ14" s="56"/>
+      <c r="DR14" s="56"/>
+      <c r="DS14" s="56"/>
+      <c r="DT14" s="56"/>
+      <c r="DU14" s="56"/>
+      <c r="DV14" s="56"/>
+      <c r="DW14" s="56"/>
+      <c r="DX14" s="56"/>
+      <c r="DY14" s="56"/>
+      <c r="DZ14" s="56"/>
+      <c r="EA14" s="56"/>
+      <c r="EB14" s="56"/>
+      <c r="EC14" s="56"/>
+      <c r="ED14" s="56"/>
+      <c r="EE14" s="56"/>
+      <c r="EF14" s="56"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="55"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="55"/>
-      <c r="M14" s="55"/>
-      <c r="N14" s="55"/>
-      <c r="O14" s="55"/>
-      <c r="P14" s="55"/>
-      <c r="Q14" s="55"/>
-      <c r="R14" s="55"/>
-      <c r="S14" s="55"/>
-      <c r="T14" s="55"/>
-      <c r="U14" s="55"/>
-      <c r="V14" s="55"/>
-      <c r="W14" s="55"/>
-      <c r="X14" s="55"/>
-      <c r="Y14" s="55"/>
-      <c r="Z14" s="55"/>
-      <c r="AA14" s="55"/>
-      <c r="AB14" s="55"/>
-      <c r="AC14" s="55"/>
-      <c r="AD14" s="55"/>
-      <c r="AE14" s="55"/>
-      <c r="AF14" s="55"/>
-      <c r="AG14" s="55"/>
-      <c r="AH14" s="55"/>
-      <c r="AI14" s="55"/>
-      <c r="AJ14" s="55"/>
-      <c r="AK14" s="55"/>
-      <c r="AL14" s="55"/>
-      <c r="AM14" s="55"/>
-      <c r="AN14" s="55"/>
-      <c r="AO14" s="55"/>
-      <c r="AP14" s="55"/>
-      <c r="AQ14" s="55"/>
-      <c r="AR14" s="55"/>
-      <c r="AS14" s="55"/>
-      <c r="AT14" s="55"/>
-      <c r="AU14" s="55"/>
-      <c r="AV14" s="55"/>
-      <c r="AW14" s="55"/>
-      <c r="AX14" s="55"/>
-      <c r="AY14" s="55"/>
-      <c r="AZ14" s="55"/>
-      <c r="BA14" s="55"/>
-      <c r="BB14" s="55"/>
-      <c r="BC14" s="55"/>
-      <c r="BD14" s="55"/>
-      <c r="BE14" s="55"/>
-      <c r="BF14" s="55"/>
-      <c r="BG14" s="55"/>
-      <c r="BH14" s="55"/>
-      <c r="BI14" s="55"/>
-      <c r="BJ14" s="55"/>
-      <c r="BK14" s="55"/>
-      <c r="BL14" s="55"/>
-      <c r="BM14" s="55"/>
-      <c r="BN14" s="55"/>
-      <c r="BO14" s="55"/>
-      <c r="BP14" s="55"/>
-      <c r="BQ14" s="55"/>
-      <c r="BR14" s="55"/>
-      <c r="BS14" s="55"/>
-      <c r="BT14" s="55"/>
-      <c r="BU14" s="55"/>
-      <c r="BV14" s="55"/>
-      <c r="BW14" s="55"/>
-      <c r="BX14" s="55"/>
-      <c r="BY14" s="55"/>
-      <c r="BZ14" s="55"/>
-      <c r="CA14" s="55"/>
-      <c r="CB14" s="55"/>
-      <c r="CC14" s="55"/>
-      <c r="CD14" s="55"/>
-      <c r="CE14" s="55"/>
-      <c r="CF14" s="55"/>
-      <c r="CG14" s="55"/>
-      <c r="CH14" s="55"/>
-      <c r="CI14" s="55"/>
-      <c r="CJ14" s="55"/>
-      <c r="CK14" s="55"/>
-      <c r="CL14" s="55"/>
-      <c r="CM14" s="55"/>
-      <c r="CN14" s="55"/>
-      <c r="CO14" s="55"/>
-      <c r="CP14" s="55"/>
-      <c r="CQ14" s="55"/>
-      <c r="CR14" s="55"/>
-      <c r="CS14" s="55"/>
-      <c r="CT14" s="55"/>
-      <c r="CU14" s="55"/>
-      <c r="CV14" s="55"/>
-      <c r="CW14" s="55"/>
-      <c r="CX14" s="55"/>
-      <c r="CY14" s="55"/>
-      <c r="CZ14" s="55"/>
-      <c r="DA14" s="55"/>
-      <c r="DB14" s="55"/>
-      <c r="DC14" s="55"/>
-      <c r="DD14" s="55"/>
-      <c r="DE14" s="55"/>
-      <c r="DF14" s="55"/>
-      <c r="DG14" s="55"/>
-      <c r="DH14" s="55"/>
-      <c r="DI14" s="55"/>
-      <c r="DJ14" s="55"/>
-      <c r="DK14" s="55"/>
-      <c r="DL14" s="55"/>
-      <c r="DM14" s="55"/>
-      <c r="DN14" s="55"/>
-      <c r="DO14" s="55"/>
-      <c r="DP14" s="55"/>
-      <c r="DQ14" s="55"/>
-      <c r="DR14" s="55"/>
-      <c r="DS14" s="55"/>
-      <c r="DT14" s="55"/>
-      <c r="DU14" s="55"/>
-      <c r="DV14" s="55"/>
-      <c r="DW14" s="55"/>
-      <c r="DX14" s="55"/>
-      <c r="DY14" s="55"/>
-      <c r="DZ14" s="55"/>
-      <c r="EA14" s="55"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="55"/>
-      <c r="L15" s="55"/>
-      <c r="M15" s="55"/>
-      <c r="N15" s="55"/>
-      <c r="O15" s="55"/>
-      <c r="P15" s="55"/>
-      <c r="Q15" s="55"/>
-      <c r="R15" s="55"/>
-      <c r="S15" s="55"/>
-      <c r="T15" s="55"/>
-      <c r="U15" s="55"/>
-      <c r="V15" s="55"/>
-      <c r="W15" s="55"/>
-      <c r="X15" s="55"/>
-      <c r="Y15" s="55"/>
-      <c r="Z15" s="55"/>
-      <c r="AA15" s="55"/>
-      <c r="AB15" s="55"/>
-      <c r="AC15" s="55"/>
-      <c r="AD15" s="55"/>
-      <c r="AE15" s="55"/>
-      <c r="AF15" s="55"/>
-      <c r="AG15" s="55"/>
-      <c r="AH15" s="55"/>
-      <c r="AI15" s="55"/>
-      <c r="AJ15" s="55"/>
-      <c r="AK15" s="55"/>
-      <c r="AL15" s="55"/>
-      <c r="AM15" s="55"/>
-      <c r="AN15" s="55"/>
-      <c r="AO15" s="55"/>
-      <c r="AP15" s="55"/>
-      <c r="AQ15" s="55"/>
-      <c r="AR15" s="55"/>
-      <c r="AS15" s="55"/>
-      <c r="AT15" s="55"/>
-      <c r="AU15" s="55"/>
-      <c r="AV15" s="55"/>
-      <c r="AW15" s="55"/>
-      <c r="AX15" s="55"/>
-      <c r="AY15" s="55"/>
-      <c r="AZ15" s="55"/>
-      <c r="BA15" s="55"/>
-      <c r="BB15" s="55"/>
-      <c r="BC15" s="55"/>
-      <c r="BD15" s="55"/>
-      <c r="BE15" s="55"/>
-      <c r="BF15" s="55"/>
-      <c r="BG15" s="55"/>
-      <c r="BH15" s="55"/>
-      <c r="BI15" s="55"/>
-      <c r="BJ15" s="55"/>
-      <c r="BK15" s="55"/>
-      <c r="BL15" s="55"/>
-      <c r="BM15" s="55"/>
-      <c r="BN15" s="55"/>
-      <c r="BO15" s="55"/>
-      <c r="BP15" s="55"/>
-      <c r="BQ15" s="55"/>
-      <c r="BR15" s="55"/>
-      <c r="BS15" s="55"/>
-      <c r="BT15" s="55"/>
-      <c r="BU15" s="55"/>
-      <c r="BV15" s="55"/>
-      <c r="BW15" s="55"/>
-      <c r="BX15" s="55"/>
-      <c r="BY15" s="55"/>
-      <c r="BZ15" s="55"/>
-      <c r="CA15" s="55"/>
-      <c r="CB15" s="55"/>
-      <c r="CC15" s="55"/>
-      <c r="CD15" s="55"/>
-      <c r="CE15" s="55"/>
-      <c r="CF15" s="55"/>
-      <c r="CG15" s="55"/>
-      <c r="CH15" s="55"/>
-      <c r="CI15" s="55"/>
-      <c r="CJ15" s="55"/>
-      <c r="CK15" s="55"/>
-      <c r="CL15" s="55"/>
-      <c r="CM15" s="55"/>
-      <c r="CN15" s="55"/>
-      <c r="CO15" s="55"/>
-      <c r="CP15" s="55"/>
-      <c r="CQ15" s="55"/>
-      <c r="CR15" s="55"/>
-      <c r="CS15" s="55"/>
-      <c r="CT15" s="55"/>
-      <c r="CU15" s="55"/>
-      <c r="CV15" s="55"/>
-      <c r="CW15" s="55"/>
-      <c r="CX15" s="55"/>
-      <c r="CY15" s="55"/>
-      <c r="CZ15" s="55"/>
-      <c r="DA15" s="55"/>
-      <c r="DB15" s="55"/>
-      <c r="DC15" s="55"/>
-      <c r="DD15" s="55"/>
-      <c r="DE15" s="55"/>
-      <c r="DF15" s="55"/>
-      <c r="DG15" s="55"/>
-      <c r="DH15" s="55"/>
-      <c r="DI15" s="55"/>
-      <c r="DJ15" s="55"/>
-      <c r="DK15" s="55"/>
-      <c r="DL15" s="55"/>
-      <c r="DM15" s="55"/>
-      <c r="DN15" s="55"/>
-      <c r="DO15" s="55"/>
-      <c r="DP15" s="55"/>
-      <c r="DQ15" s="55"/>
-      <c r="DR15" s="55"/>
-      <c r="DS15" s="55"/>
-      <c r="DT15" s="55"/>
-      <c r="DU15" s="55"/>
-      <c r="DV15" s="55"/>
-      <c r="DW15" s="55"/>
-      <c r="DX15" s="55"/>
-      <c r="DY15" s="55"/>
-      <c r="DZ15" s="55"/>
-      <c r="EA15" s="55"/>
+    <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="56"/>
+      <c r="H15" s="55" t="n">
+        <v>4366</v>
+      </c>
+      <c r="I15" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="J15" s="55" t="n">
+        <v>5</v>
+      </c>
+      <c r="K15" s="56"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="55" t="n">
+        <v>34</v>
+      </c>
+      <c r="N15" s="56"/>
+      <c r="O15" s="56"/>
+      <c r="P15" s="56"/>
+      <c r="Q15" s="56"/>
+      <c r="R15" s="56"/>
+      <c r="S15" s="56"/>
+      <c r="T15" s="56"/>
+      <c r="U15" s="57" t="s">
+        <v>286</v>
+      </c>
+      <c r="V15" s="56"/>
+      <c r="W15" s="56"/>
+      <c r="X15" s="56"/>
+      <c r="Y15" s="56"/>
+      <c r="Z15" s="56"/>
+      <c r="AA15" s="56"/>
+      <c r="AB15" s="56"/>
+      <c r="AC15" s="56"/>
+      <c r="AD15" s="56"/>
+      <c r="AE15" s="56"/>
+      <c r="AF15" s="56"/>
+      <c r="AG15" s="56"/>
+      <c r="AH15" s="56"/>
+      <c r="AI15" s="56"/>
+      <c r="AJ15" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AK15" s="56"/>
+      <c r="AL15" s="56"/>
+      <c r="AM15" s="56"/>
+      <c r="AN15" s="56"/>
+      <c r="AO15" s="56"/>
+      <c r="AP15" s="56"/>
+      <c r="AQ15" s="56"/>
+      <c r="AR15" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS15" s="55" t="n">
+        <v>7</v>
+      </c>
+      <c r="AT15" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="AU15" s="56"/>
+      <c r="AV15" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW15" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX15" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AY15" s="56"/>
+      <c r="AZ15" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA15" s="55" t="n">
+        <v>18</v>
+      </c>
+      <c r="BB15" s="56"/>
+      <c r="BC15" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="BD15" s="56"/>
+      <c r="BE15" s="56"/>
+      <c r="BF15" s="56"/>
+      <c r="BG15" s="56"/>
+      <c r="BH15" s="56"/>
+      <c r="BI15" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ15" s="55" t="n">
+        <v>18</v>
+      </c>
+      <c r="BK15" s="57" t="s">
+        <v>287</v>
+      </c>
+      <c r="BL15" s="56"/>
+      <c r="BM15" s="56"/>
+      <c r="BN15" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO15" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="BP15" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="BQ15" s="55" t="n">
+        <v>7</v>
+      </c>
+      <c r="BR15" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BS15" s="56"/>
+      <c r="BT15" s="56"/>
+      <c r="BU15" s="56"/>
+      <c r="BV15" s="56"/>
+      <c r="BW15" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="BX15" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BY15" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="BZ15" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="CA15" s="55" t="n">
+        <v>4</v>
+      </c>
+      <c r="CB15" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC15" s="55" t="n">
+        <v>90.44</v>
+      </c>
+      <c r="CD15" s="55" t="n">
+        <v>140.67</v>
+      </c>
+      <c r="CE15" s="55" t="n">
+        <v>5.34</v>
+      </c>
+      <c r="CF15" s="55" t="n">
+        <v>43</v>
+      </c>
+      <c r="CG15" s="55" t="n">
+        <v>279.45</v>
+      </c>
+      <c r="CH15" s="56"/>
+      <c r="CI15" s="56"/>
+      <c r="CJ15" s="55" t="n">
+        <v>3</v>
+      </c>
+      <c r="CK15" s="56"/>
+      <c r="CL15" s="55" t="n">
+        <v>30</v>
+      </c>
+      <c r="CM15" s="55" t="n">
+        <v>5</v>
+      </c>
+      <c r="CN15" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="CO15" s="56"/>
+      <c r="CP15" s="56"/>
+      <c r="CQ15" s="56"/>
+      <c r="CR15" s="56"/>
+      <c r="CS15" s="55" t="n">
+        <v>22</v>
+      </c>
+      <c r="CT15" s="55" t="n">
+        <v>6</v>
+      </c>
+      <c r="CU15" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="CV15" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW15" s="57" t="s">
+        <v>300</v>
+      </c>
+      <c r="CX15" s="56"/>
+      <c r="CY15" s="56"/>
+      <c r="CZ15" s="56"/>
+      <c r="DA15" s="55" t="n">
+        <v>2</v>
+      </c>
+      <c r="DB15" s="56"/>
+      <c r="DC15" s="55" t="n">
+        <v>12</v>
+      </c>
+      <c r="DD15" s="56"/>
+      <c r="DE15" s="56"/>
+      <c r="DF15" s="56"/>
+      <c r="DG15" s="56"/>
+      <c r="DH15" s="55" t="n">
+        <v>107242</v>
+      </c>
+      <c r="DI15" s="57" t="s">
+        <v>289</v>
+      </c>
+      <c r="DJ15" s="55" t="n">
+        <v>107242</v>
+      </c>
+      <c r="DK15" s="56"/>
+      <c r="DL15" s="57" t="s">
+        <v>300</v>
+      </c>
+      <c r="DM15" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DN15" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DO15" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="DP15" s="56"/>
+      <c r="DQ15" s="56"/>
+      <c r="DR15" s="56"/>
+      <c r="DS15" s="56"/>
+      <c r="DT15" s="56"/>
+      <c r="DU15" s="56"/>
+      <c r="DV15" s="56"/>
+      <c r="DW15" s="56"/>
+      <c r="DX15" s="56"/>
+      <c r="DY15" s="56"/>
+      <c r="DZ15" s="56"/>
+      <c r="EA15" s="56"/>
+      <c r="EB15" s="56"/>
+      <c r="EC15" s="56"/>
+      <c r="ED15" s="56"/>
+      <c r="EE15" s="56"/>
+      <c r="EF15" s="56"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="55"/>
-      <c r="L16" s="55"/>
-      <c r="M16" s="55"/>
-      <c r="N16" s="55"/>
-      <c r="O16" s="55"/>
-      <c r="P16" s="55"/>
-      <c r="Q16" s="55"/>
-      <c r="R16" s="55"/>
-      <c r="S16" s="55"/>
-      <c r="T16" s="55"/>
-      <c r="U16" s="55"/>
-      <c r="V16" s="55"/>
-      <c r="W16" s="55"/>
-      <c r="X16" s="55"/>
-      <c r="Y16" s="55"/>
-      <c r="Z16" s="55"/>
-      <c r="AA16" s="55"/>
-      <c r="AB16" s="55"/>
-      <c r="AC16" s="55"/>
-      <c r="AD16" s="55"/>
-      <c r="AE16" s="55"/>
-      <c r="AF16" s="55"/>
-      <c r="AG16" s="55"/>
-      <c r="AH16" s="55"/>
-      <c r="AI16" s="55"/>
-      <c r="AJ16" s="55"/>
-      <c r="AK16" s="55"/>
-      <c r="AL16" s="55"/>
-      <c r="AM16" s="55"/>
-      <c r="AN16" s="55"/>
-      <c r="AO16" s="55"/>
-      <c r="AP16" s="55"/>
-      <c r="AQ16" s="55"/>
-      <c r="AR16" s="55"/>
-      <c r="AS16" s="55"/>
-      <c r="AT16" s="55"/>
-      <c r="AU16" s="55"/>
-      <c r="AV16" s="55"/>
-      <c r="AW16" s="55"/>
-      <c r="AX16" s="55"/>
-      <c r="AY16" s="55"/>
-      <c r="AZ16" s="55"/>
-      <c r="BA16" s="55"/>
-      <c r="BB16" s="55"/>
-      <c r="BC16" s="55"/>
-      <c r="BD16" s="55"/>
-      <c r="BE16" s="55"/>
-      <c r="BF16" s="55"/>
-      <c r="BG16" s="55"/>
-      <c r="BH16" s="55"/>
-      <c r="BI16" s="55"/>
-      <c r="BJ16" s="55"/>
-      <c r="BK16" s="55"/>
-      <c r="BL16" s="55"/>
-      <c r="BM16" s="55"/>
-      <c r="BN16" s="55"/>
-      <c r="BO16" s="55"/>
-      <c r="BP16" s="55"/>
-      <c r="BQ16" s="55"/>
-      <c r="BR16" s="55"/>
-      <c r="BS16" s="55"/>
-      <c r="BT16" s="55"/>
-      <c r="BU16" s="55"/>
-      <c r="BV16" s="55"/>
-      <c r="BW16" s="55"/>
-      <c r="BX16" s="55"/>
-      <c r="BY16" s="55"/>
-      <c r="BZ16" s="55"/>
-      <c r="CA16" s="55"/>
-      <c r="CB16" s="55"/>
-      <c r="CC16" s="55"/>
-      <c r="CD16" s="55"/>
-      <c r="CE16" s="55"/>
-      <c r="CF16" s="55"/>
-      <c r="CG16" s="55"/>
-      <c r="CH16" s="55"/>
-      <c r="CI16" s="55"/>
-      <c r="CJ16" s="55"/>
-      <c r="CK16" s="55"/>
-      <c r="CL16" s="55"/>
-      <c r="CM16" s="55"/>
-      <c r="CN16" s="55"/>
-      <c r="CO16" s="55"/>
-      <c r="CP16" s="55"/>
-      <c r="CQ16" s="55"/>
-      <c r="CR16" s="55"/>
-      <c r="CS16" s="55"/>
-      <c r="CT16" s="55"/>
-      <c r="CU16" s="55"/>
-      <c r="CV16" s="55"/>
-      <c r="CW16" s="55"/>
-      <c r="CX16" s="55"/>
-      <c r="CY16" s="55"/>
-      <c r="CZ16" s="55"/>
-      <c r="DA16" s="55"/>
-      <c r="DB16" s="55"/>
-      <c r="DC16" s="55"/>
-      <c r="DD16" s="55"/>
-      <c r="DE16" s="55"/>
-      <c r="DF16" s="55"/>
-      <c r="DG16" s="55"/>
-      <c r="DH16" s="55"/>
-      <c r="DI16" s="55"/>
-      <c r="DJ16" s="55"/>
-      <c r="DK16" s="55"/>
-      <c r="DL16" s="55"/>
-      <c r="DM16" s="55"/>
-      <c r="DN16" s="55"/>
-      <c r="DO16" s="55"/>
-      <c r="DP16" s="55"/>
-      <c r="DQ16" s="55"/>
-      <c r="DR16" s="55"/>
-      <c r="DS16" s="55"/>
-      <c r="DT16" s="55"/>
-      <c r="DU16" s="55"/>
-      <c r="DV16" s="55"/>
-      <c r="DW16" s="55"/>
-      <c r="DX16" s="55"/>
-      <c r="DY16" s="55"/>
-      <c r="DZ16" s="55"/>
-      <c r="EA16" s="55"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="58"/>
+      <c r="N16" s="58"/>
+      <c r="O16" s="58"/>
+      <c r="P16" s="58"/>
+      <c r="Q16" s="58"/>
+      <c r="R16" s="58"/>
+      <c r="S16" s="58"/>
+      <c r="T16" s="58"/>
+      <c r="U16" s="58"/>
+      <c r="V16" s="58"/>
+      <c r="W16" s="58"/>
+      <c r="X16" s="58"/>
+      <c r="Y16" s="58"/>
+      <c r="Z16" s="58"/>
+      <c r="AA16" s="58"/>
+      <c r="AB16" s="58"/>
+      <c r="AC16" s="58"/>
+      <c r="AD16" s="58"/>
+      <c r="AE16" s="58"/>
+      <c r="AF16" s="58"/>
+      <c r="AG16" s="58"/>
+      <c r="AH16" s="58"/>
+      <c r="AI16" s="58"/>
+      <c r="AJ16" s="58"/>
+      <c r="AK16" s="58"/>
+      <c r="AL16" s="58"/>
+      <c r="AM16" s="58"/>
+      <c r="AN16" s="58"/>
+      <c r="AO16" s="58"/>
+      <c r="AP16" s="58"/>
+      <c r="AQ16" s="58"/>
+      <c r="AR16" s="58"/>
+      <c r="AS16" s="58"/>
+      <c r="AT16" s="58"/>
+      <c r="AU16" s="58"/>
+      <c r="AV16" s="58"/>
+      <c r="AW16" s="58"/>
+      <c r="AX16" s="58"/>
+      <c r="AY16" s="58"/>
+      <c r="AZ16" s="58"/>
+      <c r="BA16" s="58"/>
+      <c r="BB16" s="58"/>
+      <c r="BC16" s="58"/>
+      <c r="BD16" s="58"/>
+      <c r="BE16" s="58"/>
+      <c r="BF16" s="58"/>
+      <c r="BG16" s="58"/>
+      <c r="BH16" s="58"/>
+      <c r="BI16" s="58"/>
+      <c r="BJ16" s="58"/>
+      <c r="BK16" s="58"/>
+      <c r="BL16" s="58"/>
+      <c r="BM16" s="58"/>
+      <c r="BN16" s="58"/>
+      <c r="BO16" s="58"/>
+      <c r="BP16" s="58"/>
+      <c r="BQ16" s="58"/>
+      <c r="BR16" s="58"/>
+      <c r="BS16" s="58"/>
+      <c r="BT16" s="58"/>
+      <c r="BU16" s="58"/>
+      <c r="BV16" s="58"/>
+      <c r="BW16" s="58"/>
+      <c r="BX16" s="58"/>
+      <c r="BY16" s="58"/>
+      <c r="BZ16" s="58"/>
+      <c r="CA16" s="58"/>
+      <c r="CB16" s="58"/>
+      <c r="CC16" s="58"/>
+      <c r="CD16" s="58"/>
+      <c r="CE16" s="58"/>
+      <c r="CF16" s="58"/>
+      <c r="CG16" s="58"/>
+      <c r="CH16" s="58"/>
+      <c r="CI16" s="58"/>
+      <c r="CJ16" s="58"/>
+      <c r="CK16" s="58"/>
+      <c r="CL16" s="58"/>
+      <c r="CM16" s="58"/>
+      <c r="CN16" s="58"/>
+      <c r="CO16" s="58"/>
+      <c r="CP16" s="58"/>
+      <c r="CQ16" s="58"/>
+      <c r="CR16" s="58"/>
+      <c r="CS16" s="58"/>
+      <c r="CT16" s="58"/>
+      <c r="CU16" s="58"/>
+      <c r="CV16" s="58"/>
+      <c r="CW16" s="58"/>
+      <c r="CX16" s="58"/>
+      <c r="CY16" s="58"/>
+      <c r="CZ16" s="58"/>
+      <c r="DA16" s="58"/>
+      <c r="DB16" s="58"/>
+      <c r="DC16" s="58"/>
+      <c r="DD16" s="58"/>
+      <c r="DE16" s="58"/>
+      <c r="DF16" s="58"/>
+      <c r="DG16" s="58"/>
+      <c r="DH16" s="58"/>
+      <c r="DI16" s="58"/>
+      <c r="DJ16" s="58"/>
+      <c r="DK16" s="58"/>
+      <c r="DL16" s="58"/>
+      <c r="DM16" s="58"/>
+      <c r="DN16" s="58"/>
+      <c r="DO16" s="58"/>
+      <c r="DP16" s="58"/>
+      <c r="DQ16" s="58"/>
+      <c r="DR16" s="58"/>
+      <c r="DS16" s="58"/>
+      <c r="DT16" s="58"/>
+      <c r="DU16" s="58"/>
+      <c r="DV16" s="58"/>
+      <c r="DW16" s="58"/>
+      <c r="DX16" s="58"/>
+      <c r="DY16" s="58"/>
+      <c r="DZ16" s="58"/>
+      <c r="EA16" s="58"/>
     </row>
     <row r="17" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="57"/>
-      <c r="K17" s="57"/>
-      <c r="M17" s="57"/>
-      <c r="N17" s="57"/>
-      <c r="O17" s="57"/>
-      <c r="P17" s="57"/>
-      <c r="Q17" s="57"/>
-      <c r="R17" s="57"/>
-      <c r="S17" s="57"/>
-      <c r="T17" s="57"/>
-      <c r="U17" s="57"/>
-      <c r="V17" s="57"/>
-      <c r="W17" s="57"/>
-      <c r="X17" s="57"/>
-      <c r="Y17" s="57"/>
-      <c r="Z17" s="57"/>
-      <c r="AA17" s="57"/>
-      <c r="AB17" s="57"/>
-      <c r="AC17" s="57"/>
-      <c r="AD17" s="57"/>
-      <c r="AE17" s="57"/>
-      <c r="AF17" s="57"/>
-      <c r="AG17" s="57"/>
-      <c r="AH17" s="57"/>
-      <c r="AI17" s="57"/>
-      <c r="AJ17" s="57"/>
-      <c r="AK17" s="57"/>
-      <c r="AL17" s="57"/>
-      <c r="AM17" s="57"/>
-      <c r="AN17" s="57"/>
-      <c r="AO17" s="57"/>
-      <c r="AP17" s="57"/>
-      <c r="AQ17" s="57"/>
-      <c r="AR17" s="57"/>
-      <c r="AS17" s="57"/>
-      <c r="AT17" s="57"/>
-      <c r="AU17" s="57"/>
-      <c r="AV17" s="57"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
+      <c r="M17" s="59"/>
+      <c r="N17" s="59"/>
+      <c r="O17" s="59"/>
+      <c r="P17" s="59"/>
+      <c r="Q17" s="59"/>
+      <c r="R17" s="59"/>
+      <c r="S17" s="59"/>
+      <c r="T17" s="59"/>
+      <c r="U17" s="59"/>
+      <c r="V17" s="59"/>
+      <c r="W17" s="59"/>
+      <c r="X17" s="59"/>
+      <c r="Y17" s="59"/>
+      <c r="Z17" s="59"/>
+      <c r="AA17" s="59"/>
+      <c r="AB17" s="59"/>
+      <c r="AC17" s="59"/>
+      <c r="AD17" s="59"/>
+      <c r="AE17" s="59"/>
+      <c r="AF17" s="59"/>
+      <c r="AG17" s="59"/>
+      <c r="AH17" s="59"/>
+      <c r="AI17" s="59"/>
+      <c r="AJ17" s="59"/>
+      <c r="AK17" s="59"/>
+      <c r="AL17" s="59"/>
+      <c r="AM17" s="59"/>
+      <c r="AN17" s="59"/>
+      <c r="AO17" s="59"/>
+      <c r="AP17" s="59"/>
+      <c r="AQ17" s="59"/>
+      <c r="AR17" s="59"/>
+      <c r="AS17" s="59"/>
+      <c r="AT17" s="59"/>
+      <c r="AU17" s="59"/>
+      <c r="AV17" s="59"/>
       <c r="BC17" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CLDC-883: Clear dependent answers when the dependency value changes (#206)
* Failing spec

* Reset invalidated fields

* Page routing can also depend on subsection
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/2021_22_lettings_bulk_upload.xlsx
+++ b/spec/fixtures/files/2021_22_lettings_bulk_upload.xlsx
@@ -1892,8 +1892,8 @@
   </sheetPr>
   <dimension ref="A1:EF17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CB1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CU15" activeCellId="0" sqref="CU15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4138,7 +4138,7 @@
         <v>9</v>
       </c>
       <c r="CU7" s="55" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="CV7" s="55" t="n">
         <v>0</v>
@@ -4383,7 +4383,7 @@
         <v>4</v>
       </c>
       <c r="CU8" s="55" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="CV8" s="55" t="n">
         <v>0</v>
@@ -4628,7 +4628,7 @@
         <v>4</v>
       </c>
       <c r="CU9" s="55" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="CV9" s="55" t="n">
         <v>0</v>
@@ -4873,7 +4873,7 @@
         <v>4</v>
       </c>
       <c r="CU10" s="55" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="CV10" s="55" t="n">
         <v>0</v>
@@ -5118,7 +5118,7 @@
         <v>5</v>
       </c>
       <c r="CU11" s="55" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="CV11" s="55" t="n">
         <v>0</v>
@@ -5363,7 +5363,7 @@
         <v>6</v>
       </c>
       <c r="CU12" s="55" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="CV12" s="55" t="n">
         <v>0</v>
@@ -5608,7 +5608,7 @@
         <v>4</v>
       </c>
       <c r="CU13" s="55" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="CV13" s="55" t="n">
         <v>0</v>
@@ -5853,7 +5853,7 @@
         <v>8</v>
       </c>
       <c r="CU14" s="55" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="CV14" s="55" t="n">
         <v>0</v>
@@ -6100,7 +6100,7 @@
         <v>6</v>
       </c>
       <c r="CU15" s="55" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="CV15" s="55" t="n">
         <v>0</v>

</xml_diff>